<commit_message>
New path managing function and run function
</commit_message>
<xml_diff>
--- a/XC-template.xlsx
+++ b/XC-template.xlsx
@@ -1,16 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr backupFile="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25317"/>
+  <workbookPr backupFile="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="11295" windowHeight="6750" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="100" windowWidth="19140" windowHeight="14480"/>
   </bookViews>
   <sheets>
     <sheet name="xc1" sheetId="1" r:id="rId1"/>
     <sheet name="xc2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -128,29 +133,29 @@
     <t>2c</t>
   </si>
   <si>
-    <t>xc1</t>
-  </si>
-  <si>
     <t>test cross section</t>
   </si>
   <si>
     <t>1g</t>
   </si>
   <si>
-    <t>xc2</t>
-  </si>
-  <si>
     <t>2g</t>
   </si>
   <si>
     <t>Main Title</t>
+  </si>
+  <si>
+    <t>Cross Section 2</t>
+  </si>
+  <si>
+    <t>Cross Section 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -236,7 +241,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -248,7 +253,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -257,7 +262,7 @@
       <right/>
       <top/>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -265,27 +270,27 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -294,30 +299,30 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -326,46 +331,46 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -373,7 +378,7 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -381,10 +386,10 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -392,13 +397,13 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -589,7 +594,17 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -598,16 +613,20 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>xc1</c:v>
+              <c:v>Cross Section 1</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
       </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -630,22 +649,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>-10</c:v>
+                  <c:v>-10.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-5</c:v>
+                  <c:v>-5.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-5</c:v>
+                  <c:v>-5.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -657,26 +676,27 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22</c:v>
+                  <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28</c:v>
+                  <c:v>28.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22</c:v>
+                  <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>28</c:v>
+                  <c:v>28.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -700,10 +720,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-5</c:v>
+                  <c:v>-5.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -715,14 +735,15 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -750,10 +771,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -768,11 +789,12 @@
                   <c:v>33.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -798,10 +820,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>-25</c:v>
+                  <c:v>-25.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-25</c:v>
+                  <c:v>-25.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -816,49 +838,68 @@
                   <c:v>33.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="90151936"/>
-        <c:axId val="70959872"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2067308392"/>
+        <c:axId val="2067135208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="90151936"/>
+        <c:axId val="2067308392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="70959872"/>
+        <c:crossAx val="2067135208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="70959872"/>
+        <c:axId val="2067135208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90151936"/>
+        <c:crossAx val="2067308392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000002" l="0.700000000000001" r="0.700000000000001" t="0.750000000000002" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -866,7 +907,17 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -875,17 +926,20 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>xc2</c:v>
+              <c:v>Cross Section 2</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -908,22 +962,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>-5</c:v>
+                  <c:v>-5.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-7</c:v>
+                  <c:v>-7.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-5</c:v>
+                  <c:v>-5.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -935,26 +989,27 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27</c:v>
+                  <c:v>27.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27</c:v>
+                  <c:v>27.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -978,10 +1033,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-2</c:v>
+                  <c:v>-2.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -993,14 +1048,15 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>35.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35</c:v>
+                  <c:v>35.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1046,11 +1102,12 @@
                   <c:v>36.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1094,37 +1151,52 @@
                   <c:v>36.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="108305792"/>
-        <c:axId val="108307584"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2076268328"/>
+        <c:axId val="2076265192"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="108305792"/>
+        <c:axId val="2076268328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108307584"/>
+        <c:crossAx val="2076265192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="108307584"/>
+        <c:axId val="2076265192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108305792"/>
+        <c:crossAx val="2076268328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1132,12 +1204,15 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000002" l="0.700000000000001" r="0.700000000000001" t="0.750000000000002" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1497,29 +1572,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="35.83203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="21" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="11" customWidth="1"/>
-    <col min="4" max="10" width="10.5703125" style="9" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" style="14" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" style="6" customWidth="1"/>
-    <col min="13" max="16" width="10.5703125" style="9" customWidth="1"/>
-    <col min="17" max="17" width="10.5703125" style="14" customWidth="1"/>
-    <col min="18" max="18" width="22.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="9"/>
+    <col min="3" max="3" width="10.5" style="11" customWidth="1"/>
+    <col min="4" max="10" width="10.5" style="9" customWidth="1"/>
+    <col min="11" max="11" width="10.5" style="14" customWidth="1"/>
+    <col min="12" max="12" width="10.5" style="6" customWidth="1"/>
+    <col min="13" max="16" width="10.5" style="9" customWidth="1"/>
+    <col min="17" max="17" width="10.5" style="14" customWidth="1"/>
+    <col min="18" max="18" width="22.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="25" customFormat="1" ht="15">
+    <row r="1" spans="1:19" s="25" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1559,7 +1634,7 @@
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
     </row>
-    <row r="3" spans="1:19" ht="15.75">
+    <row r="3" spans="1:19" ht="15">
       <c r="A3" s="34" t="s">
         <v>21</v>
       </c>
@@ -1588,7 +1663,7 @@
       </c>
       <c r="S3" s="33"/>
     </row>
-    <row r="4" spans="1:19" ht="38.25">
+    <row r="4" spans="1:19" ht="42">
       <c r="A4" s="23" t="s">
         <v>28</v>
       </c>
@@ -1652,7 +1727,7 @@
         <v>26</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>31</v>
@@ -1683,7 +1758,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M5" s="9">
         <v>-5</v>
@@ -1714,7 +1789,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>32</v>
@@ -1744,7 +1819,7 @@
         <v>120</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="M6" s="9">
         <v>10</v>
@@ -1941,7 +2016,7 @@
       </c>
       <c r="L12" s="9"/>
     </row>
-    <row r="13" spans="1:19" ht="13.5" thickBot="1">
+    <row r="13" spans="1:19" ht="15" thickBot="1">
       <c r="A13" s="19" t="s">
         <v>7</v>
       </c>
@@ -2034,41 +2109,46 @@
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="0.75" header="0.5" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddHeader xml:space="preserve">&amp;L&amp;"-,Regular"&amp;9Draft&amp;C&amp;"Times New Roman,Bold"&amp;11 </oddHeader>
     <oddFooter>&amp;L&amp;K4D4D4DG&amp;8RADIENT&amp;"Cambria,Regular"&amp;6
 &amp;"-,Regular"&amp;K4D4D4D
 &amp;Z&amp;F\&amp;A&amp;R&amp;"-,Regular"&amp;9Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="35.83203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="21" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="11" customWidth="1"/>
-    <col min="4" max="10" width="10.5703125" style="9" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" style="14" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" style="6" customWidth="1"/>
-    <col min="13" max="16" width="10.5703125" style="9" customWidth="1"/>
-    <col min="17" max="17" width="10.5703125" style="14" customWidth="1"/>
-    <col min="18" max="18" width="22.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="9"/>
+    <col min="3" max="3" width="10.5" style="11" customWidth="1"/>
+    <col min="4" max="10" width="10.5" style="9" customWidth="1"/>
+    <col min="11" max="11" width="10.5" style="14" customWidth="1"/>
+    <col min="12" max="12" width="10.5" style="6" customWidth="1"/>
+    <col min="13" max="16" width="10.5" style="9" customWidth="1"/>
+    <col min="17" max="17" width="10.5" style="14" customWidth="1"/>
+    <col min="18" max="18" width="22.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="25" customFormat="1" ht="15">
+    <row r="1" spans="1:19" s="25" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2108,7 +2188,7 @@
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
     </row>
-    <row r="3" spans="1:19" ht="15.75">
+    <row r="3" spans="1:19" ht="15">
       <c r="A3" s="34" t="s">
         <v>21</v>
       </c>
@@ -2137,7 +2217,7 @@
       </c>
       <c r="S3" s="33"/>
     </row>
-    <row r="4" spans="1:19" ht="38.25">
+    <row r="4" spans="1:19" ht="42">
       <c r="A4" s="23" t="s">
         <v>28</v>
       </c>
@@ -2198,10 +2278,10 @@
     </row>
     <row r="5" spans="1:19">
       <c r="A5" s="21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>31</v>
@@ -2232,7 +2312,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M5" s="9">
         <v>-2</v>
@@ -2263,7 +2343,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>32</v>
@@ -2293,7 +2373,7 @@
         <v>120</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="M6" s="9">
         <v>2</v>
@@ -2490,7 +2570,7 @@
       </c>
       <c r="L12" s="9"/>
     </row>
-    <row r="13" spans="1:19" ht="13.5" thickBot="1">
+    <row r="13" spans="1:19" ht="15" thickBot="1">
       <c r="A13" s="19" t="s">
         <v>7</v>
       </c>
@@ -2582,13 +2662,18 @@
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="0.75" header="0.5" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddHeader xml:space="preserve">&amp;L&amp;"-,Regular"&amp;9Draft&amp;C&amp;"Times New Roman,Bold"&amp;11 </oddHeader>
     <oddFooter>&amp;L&amp;K4D4D4DG&amp;8RADIENT&amp;"Cambria,Regular"&amp;6
 &amp;"-,Regular"&amp;K4D4D4D
 &amp;Z&amp;F\&amp;A&amp;R&amp;"-,Regular"&amp;9Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add ROW_edge DataFrame to SectionBook class
</commit_message>
<xml_diff>
--- a/XC-template.xlsx
+++ b/XC-template.xlsx
@@ -1,16 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25317"/>
-  <workbookPr backupFile="1" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr backupFile="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="100" windowWidth="19140" windowHeight="14480"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="19140" windowHeight="14475" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="xc1" sheetId="1" r:id="rId1"/>
     <sheet name="xc2" sheetId="2" r:id="rId2"/>
+    <sheet name="xc3" sheetId="3" r:id="rId3"/>
+    <sheet name="xc4" sheetId="4" r:id="rId4"/>
+    <sheet name="xc5" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="46">
   <si>
     <t>FIELDS Template</t>
   </si>
@@ -150,12 +153,21 @@
   <si>
     <t>Cross Section 1</t>
   </si>
+  <si>
+    <t>Cross Section 3</t>
+  </si>
+  <si>
+    <t>Cross Section 4</t>
+  </si>
+  <si>
+    <t>Cross Section 5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -594,17 +606,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -619,14 +621,11 @@
         </c:strRef>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -649,22 +648,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>-10.0</c:v>
+                  <c:v>-10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-5.0</c:v>
+                  <c:v>-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-5.0</c:v>
+                  <c:v>-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -676,27 +675,26 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22.0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25.0</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22.0</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>28.0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -720,10 +718,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-5.0</c:v>
+                  <c:v>-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -735,15 +733,14 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -771,10 +768,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>25.0</c:v>
+                  <c:v>25.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25.0</c:v>
+                  <c:v>25.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -789,12 +786,11 @@
                   <c:v>33.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -820,10 +816,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>-25.0</c:v>
+                  <c:v>-25.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-25.0</c:v>
+                  <c:v>-25.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -838,52 +834,37 @@
                   <c:v>33.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="2067308392"/>
-        <c:axId val="2067135208"/>
+        <c:axId val="71157248"/>
+        <c:axId val="71158784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2067308392"/>
+        <c:axId val="71157248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2067135208"/>
+        <c:crossAx val="71158784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2067135208"/>
+        <c:axId val="71158784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2067308392"/>
+        <c:crossAx val="71157248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -891,15 +872,13 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000002" l="0.700000000000001" r="0.700000000000001" t="0.750000000000002" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000118" r="0.70000000000000118" t="0.75000000000000222" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -907,17 +886,7 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -932,14 +901,11 @@
         </c:strRef>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -962,22 +928,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>-5.0</c:v>
+                  <c:v>-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-7.0</c:v>
+                  <c:v>-7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-5.0</c:v>
+                  <c:v>-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -989,27 +955,26 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>23.0</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27.0</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32.0</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27.0</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23.0</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1033,10 +998,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>-2.0</c:v>
+                  <c:v>-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1048,15 +1013,14 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>35.0</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35.0</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1102,12 +1066,11 @@
                   <c:v>36.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1151,52 +1114,37 @@
                   <c:v>36.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="0"/>
         </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="2076268328"/>
-        <c:axId val="2076265192"/>
+        <c:axId val="118545408"/>
+        <c:axId val="120738560"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2076268328"/>
+        <c:axId val="118545408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076265192"/>
+        <c:crossAx val="120738560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2076265192"/>
+        <c:axId val="120738560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2076268328"/>
+        <c:crossAx val="118545408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1204,15 +1152,853 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000002" l="0.700000000000001" r="0.700000000000001" t="0.750000000000002" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000222" l="0.70000000000000118" r="0.70000000000000118" t="0.75000000000000222" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:strRef>
+          <c:f>'xc3'!$B$5</c:f>
+          <c:strCache>
+            <c:ptCount val="1"/>
+            <c:pt idx="0">
+              <c:v>Cross Section 3</c:v>
+            </c:pt>
+          </c:strCache>
+        </c:strRef>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Conductor Coordinates</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'xc3'!$D$5:$D$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>-12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'xc3'!$E$5:$E$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Ground Wire Coordinates</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="7"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'xc3'!$M$5:$M$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'xc3'!$N$5:$N$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Right ROW Edge</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'xc3'!$S$7:$S$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>25.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'xc3'!$R$5:$R$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>29.400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Left ROW Edge</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'xc3'!$S$5:$S$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-25.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-25.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'xc3'!$R$5:$R$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>29.400000000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="120785920"/>
+        <c:axId val="120787712"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="120785920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="120787712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="120787712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="120785920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000244" l="0.7000000000000014" r="0.7000000000000014" t="0.75000000000000244" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:strRef>
+          <c:f>'xc4'!$B$5</c:f>
+          <c:strCache>
+            <c:ptCount val="1"/>
+            <c:pt idx="0">
+              <c:v>Cross Section 4</c:v>
+            </c:pt>
+          </c:strCache>
+        </c:strRef>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Conductor Coordinates</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'xc4'!$D$5:$D$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'xc4'!$E$5:$E$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Ground Wire Coordinates</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="7"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'xc4'!$M$5:$M$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'xc4'!$N$5:$N$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Right ROW Edge</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'xc4'!$S$7:$S$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>25.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'xc4'!$R$5:$R$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>35.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Left ROW Edge</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'xc4'!$S$5:$S$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-25.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-25.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'xc4'!$R$5:$R$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>35.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="129738624"/>
+        <c:axId val="129740160"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="129738624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="129740160"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="129740160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="129738624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000266" l="0.70000000000000162" r="0.70000000000000162" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:strRef>
+          <c:f>'xc5'!$B$5</c:f>
+          <c:strCache>
+            <c:ptCount val="1"/>
+            <c:pt idx="0">
+              <c:v>Cross Section 5</c:v>
+            </c:pt>
+          </c:strCache>
+        </c:strRef>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Conductor Coordinates</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'xc5'!$D$5:$D$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'xc5'!$E$5:$E$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Ground Wire Coordinates</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="7"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'xc5'!$M$5:$M$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'xc5'!$N$5:$N$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Right ROW Edge</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'xc5'!$S$7:$S$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>25.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'xc5'!$R$5:$R$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>35.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Left ROW Edge</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'xc5'!$S$5:$S$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-25.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-25.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'xc5'!$R$5:$R$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>35.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="130069248"/>
+        <c:axId val="130070784"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="130069248"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="130070784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="130070784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="130069248"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000289" l="0.70000000000000162" r="0.70000000000000162" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1254,6 +2040,111 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1572,29 +2463,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="35.83203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="35.85546875" style="2" customWidth="1"/>
     <col min="2" max="2" width="21" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.5" style="11" customWidth="1"/>
-    <col min="4" max="10" width="10.5" style="9" customWidth="1"/>
-    <col min="11" max="11" width="10.5" style="14" customWidth="1"/>
-    <col min="12" max="12" width="10.5" style="6" customWidth="1"/>
-    <col min="13" max="16" width="10.5" style="9" customWidth="1"/>
-    <col min="17" max="17" width="10.5" style="14" customWidth="1"/>
-    <col min="18" max="18" width="22.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.83203125" style="9"/>
+    <col min="3" max="3" width="10.42578125" style="11" customWidth="1"/>
+    <col min="4" max="10" width="10.42578125" style="9" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" style="14" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" style="6" customWidth="1"/>
+    <col min="13" max="16" width="10.42578125" style="9" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" style="14" customWidth="1"/>
+    <col min="18" max="18" width="22.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.85546875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="25" customFormat="1">
+    <row r="1" spans="1:19" s="25" customFormat="1" ht="15">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1634,7 +2525,7 @@
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
     </row>
-    <row r="3" spans="1:19" ht="15">
+    <row r="3" spans="1:19" ht="15.75">
       <c r="A3" s="34" t="s">
         <v>21</v>
       </c>
@@ -1663,7 +2554,7 @@
       </c>
       <c r="S3" s="33"/>
     </row>
-    <row r="4" spans="1:19" ht="42">
+    <row r="4" spans="1:19" ht="38.25">
       <c r="A4" s="23" t="s">
         <v>28</v>
       </c>
@@ -1781,7 +2672,7 @@
       </c>
       <c r="S5" s="28">
         <f>B12</f>
-        <v>-25</v>
+        <v>-25.5</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -1841,7 +2732,7 @@
       </c>
       <c r="S6" s="28">
         <f>B12</f>
-        <v>-25</v>
+        <v>-25.5</v>
       </c>
     </row>
     <row r="7" spans="1:19">
@@ -1882,7 +2773,7 @@
       <c r="R7" s="28"/>
       <c r="S7" s="28">
         <f>B13</f>
-        <v>25</v>
+        <v>25.5</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -1923,7 +2814,7 @@
       <c r="R8" s="28"/>
       <c r="S8" s="28">
         <f>B13</f>
-        <v>25</v>
+        <v>25.5</v>
       </c>
     </row>
     <row r="9" spans="1:19">
@@ -2012,16 +2903,16 @@
         <v>5</v>
       </c>
       <c r="B12" s="17">
-        <v>-25</v>
+        <v>-25.5</v>
       </c>
       <c r="L12" s="9"/>
     </row>
-    <row r="13" spans="1:19" ht="15" thickBot="1">
+    <row r="13" spans="1:19" ht="13.5" thickBot="1">
       <c r="A13" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="20">
-        <v>25</v>
+        <v>25.5</v>
       </c>
       <c r="C13" s="12"/>
       <c r="D13" s="8"/>
@@ -2126,29 +3017,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="35.83203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="35.85546875" style="2" customWidth="1"/>
     <col min="2" max="2" width="21" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.5" style="11" customWidth="1"/>
-    <col min="4" max="10" width="10.5" style="9" customWidth="1"/>
-    <col min="11" max="11" width="10.5" style="14" customWidth="1"/>
-    <col min="12" max="12" width="10.5" style="6" customWidth="1"/>
-    <col min="13" max="16" width="10.5" style="9" customWidth="1"/>
-    <col min="17" max="17" width="10.5" style="14" customWidth="1"/>
-    <col min="18" max="18" width="22.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.83203125" style="9"/>
+    <col min="3" max="3" width="10.42578125" style="11" customWidth="1"/>
+    <col min="4" max="10" width="10.42578125" style="9" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" style="14" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" style="6" customWidth="1"/>
+    <col min="13" max="16" width="10.42578125" style="9" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" style="14" customWidth="1"/>
+    <col min="18" max="18" width="22.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.85546875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="25" customFormat="1">
+    <row r="1" spans="1:19" s="25" customFormat="1" ht="15">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2188,7 +3079,7 @@
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
     </row>
-    <row r="3" spans="1:19" ht="15">
+    <row r="3" spans="1:19" ht="15.75">
       <c r="A3" s="34" t="s">
         <v>21</v>
       </c>
@@ -2217,7 +3108,7 @@
       </c>
       <c r="S3" s="33"/>
     </row>
-    <row r="4" spans="1:19" ht="42">
+    <row r="4" spans="1:19" ht="38.25">
       <c r="A4" s="23" t="s">
         <v>28</v>
       </c>
@@ -2570,7 +3461,7 @@
       </c>
       <c r="L12" s="9"/>
     </row>
-    <row r="13" spans="1:19" ht="15" thickBot="1">
+    <row r="13" spans="1:19" ht="13.5" thickBot="1">
       <c r="A13" s="19" t="s">
         <v>7</v>
       </c>
@@ -2676,4 +3567,1648 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:S25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="35.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="21" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="11" customWidth="1"/>
+    <col min="4" max="10" width="10.42578125" style="9" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" style="14" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" style="6" customWidth="1"/>
+    <col min="13" max="16" width="10.42578125" style="9" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" style="14" customWidth="1"/>
+    <col min="18" max="18" width="22.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.85546875" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="25" customFormat="1" ht="15">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:19" s="26" customFormat="1">
+      <c r="A2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+    </row>
+    <row r="3" spans="1:19" ht="15.75">
+      <c r="A3" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="35"/>
+      <c r="C3" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="S3" s="33"/>
+    </row>
+    <row r="4" spans="1:19" ht="38.25">
+      <c r="A4" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q4" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="R4" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="S4" s="27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="9">
+        <v>-12</v>
+      </c>
+      <c r="E5" s="9">
+        <v>23</v>
+      </c>
+      <c r="F5" s="9">
+        <v>1</v>
+      </c>
+      <c r="G5" s="9">
+        <v>1</v>
+      </c>
+      <c r="H5" s="9">
+        <f>F5*G5</f>
+        <v>1</v>
+      </c>
+      <c r="I5" s="9">
+        <v>500</v>
+      </c>
+      <c r="J5" s="9">
+        <v>100</v>
+      </c>
+      <c r="K5" s="14">
+        <v>0</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="M5" s="9">
+        <v>-10</v>
+      </c>
+      <c r="N5" s="9">
+        <v>28</v>
+      </c>
+      <c r="O5" s="9">
+        <v>1</v>
+      </c>
+      <c r="P5" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="14">
+        <v>0</v>
+      </c>
+      <c r="R5" s="28">
+        <f>MAX(E5:E25,N5:N25)*1.05</f>
+        <v>29.400000000000002</v>
+      </c>
+      <c r="S5" s="28">
+        <f>B12</f>
+        <v>-25.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="9">
+        <v>-8</v>
+      </c>
+      <c r="E6" s="9">
+        <v>23</v>
+      </c>
+      <c r="F6" s="9">
+        <v>1</v>
+      </c>
+      <c r="G6" s="9">
+        <v>1</v>
+      </c>
+      <c r="H6" s="9">
+        <v>1</v>
+      </c>
+      <c r="I6" s="9">
+        <v>500</v>
+      </c>
+      <c r="J6" s="9">
+        <v>100</v>
+      </c>
+      <c r="K6" s="14">
+        <v>120</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="M6" s="9">
+        <v>10</v>
+      </c>
+      <c r="N6" s="9">
+        <v>28</v>
+      </c>
+      <c r="O6" s="9">
+        <v>1</v>
+      </c>
+      <c r="P6" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="14">
+        <v>0</v>
+      </c>
+      <c r="R6" s="28">
+        <v>0</v>
+      </c>
+      <c r="S6" s="28">
+        <f>B12</f>
+        <v>-25.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="18">
+        <v>60</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="8">
+        <v>-4</v>
+      </c>
+      <c r="E7" s="8">
+        <v>23</v>
+      </c>
+      <c r="F7" s="8">
+        <v>1</v>
+      </c>
+      <c r="G7" s="8">
+        <v>1</v>
+      </c>
+      <c r="H7" s="8">
+        <v>1</v>
+      </c>
+      <c r="I7" s="8">
+        <v>500</v>
+      </c>
+      <c r="J7" s="8">
+        <v>100</v>
+      </c>
+      <c r="K7" s="15">
+        <v>240</v>
+      </c>
+      <c r="L7" s="9"/>
+      <c r="R7" s="28"/>
+      <c r="S7" s="28">
+        <f>B13</f>
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="A8" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="18">
+        <v>100</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="9">
+        <v>4</v>
+      </c>
+      <c r="E8" s="9">
+        <v>23</v>
+      </c>
+      <c r="F8" s="9">
+        <v>1</v>
+      </c>
+      <c r="G8" s="9">
+        <v>1</v>
+      </c>
+      <c r="H8" s="9">
+        <v>1</v>
+      </c>
+      <c r="I8" s="9">
+        <v>500</v>
+      </c>
+      <c r="J8" s="9">
+        <v>100</v>
+      </c>
+      <c r="K8" s="14">
+        <v>0</v>
+      </c>
+      <c r="L8" s="9"/>
+      <c r="R8" s="28"/>
+      <c r="S8" s="28">
+        <f>B13</f>
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="A9" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="17">
+        <v>50</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="9">
+        <v>8</v>
+      </c>
+      <c r="E9" s="9">
+        <v>23</v>
+      </c>
+      <c r="F9" s="9">
+        <v>1</v>
+      </c>
+      <c r="G9" s="9">
+        <v>1</v>
+      </c>
+      <c r="H9" s="9">
+        <v>1</v>
+      </c>
+      <c r="I9" s="9">
+        <v>500</v>
+      </c>
+      <c r="J9" s="9">
+        <v>100</v>
+      </c>
+      <c r="K9" s="14">
+        <v>120</v>
+      </c>
+      <c r="L9" s="9"/>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="A10" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="17">
+        <v>1</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="8">
+        <v>12</v>
+      </c>
+      <c r="E10" s="8">
+        <v>23</v>
+      </c>
+      <c r="F10" s="8">
+        <v>1</v>
+      </c>
+      <c r="G10" s="8">
+        <v>1</v>
+      </c>
+      <c r="H10" s="8">
+        <v>1</v>
+      </c>
+      <c r="I10" s="8">
+        <v>500</v>
+      </c>
+      <c r="J10" s="8">
+        <v>100</v>
+      </c>
+      <c r="K10" s="15">
+        <v>240</v>
+      </c>
+      <c r="L10" s="9"/>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="A11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="18">
+        <v>3</v>
+      </c>
+      <c r="L11" s="9"/>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="A12" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="17">
+        <v>-25.5</v>
+      </c>
+      <c r="L12" s="9"/>
+    </row>
+    <row r="13" spans="1:19" ht="13.5" thickBot="1">
+      <c r="A13" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="20">
+        <v>25.5</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="1:19" ht="12.75" customHeight="1">
+      <c r="A14" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="37"/>
+      <c r="L14" s="9"/>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" s="38"/>
+      <c r="B15" s="39"/>
+      <c r="L15" s="9"/>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="C16" s="12"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="9"/>
+    </row>
+    <row r="17" spans="3:12">
+      <c r="L17" s="9"/>
+    </row>
+    <row r="18" spans="3:12">
+      <c r="L18" s="9"/>
+    </row>
+    <row r="19" spans="3:12">
+      <c r="C19" s="12"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="9"/>
+    </row>
+    <row r="22" spans="3:12">
+      <c r="C22" s="12"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="15"/>
+    </row>
+    <row r="25" spans="3:12">
+      <c r="C25" s="12"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:K3"/>
+    <mergeCell ref="L3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="A14:B15"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="0.75" header="0.5" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <headerFooter>
+    <oddHeader xml:space="preserve">&amp;L&amp;"-,Regular"&amp;9Draft&amp;C&amp;"Times New Roman,Bold"&amp;11 </oddHeader>
+    <oddFooter>&amp;L&amp;K4D4D4DG&amp;8RADIENT&amp;"Cambria,Regular"&amp;6
+&amp;"-,Regular"&amp;K4D4D4D
+&amp;Z&amp;F\&amp;A&amp;R&amp;"-,Regular"&amp;9Page &amp;P of &amp;N</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:S25"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="35.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="21" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="11" customWidth="1"/>
+    <col min="4" max="10" width="10.42578125" style="9" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" style="14" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" style="6" customWidth="1"/>
+    <col min="13" max="16" width="10.42578125" style="9" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" style="14" customWidth="1"/>
+    <col min="18" max="18" width="22.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.85546875" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="25" customFormat="1" ht="15">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:19" s="26" customFormat="1">
+      <c r="A2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+    </row>
+    <row r="3" spans="1:19" ht="15.75">
+      <c r="A3" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="35"/>
+      <c r="C3" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="S3" s="33"/>
+    </row>
+    <row r="4" spans="1:19" ht="38.25">
+      <c r="A4" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q4" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="R4" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="S4" s="27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="9">
+        <v>-10</v>
+      </c>
+      <c r="E5" s="9">
+        <v>20</v>
+      </c>
+      <c r="F5" s="9">
+        <v>1</v>
+      </c>
+      <c r="G5" s="9">
+        <v>1</v>
+      </c>
+      <c r="H5" s="9">
+        <f>F5*G5</f>
+        <v>1</v>
+      </c>
+      <c r="I5" s="9">
+        <v>500</v>
+      </c>
+      <c r="J5" s="9">
+        <v>100</v>
+      </c>
+      <c r="K5" s="14">
+        <v>0</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="M5" s="9">
+        <v>-10</v>
+      </c>
+      <c r="N5" s="9">
+        <v>34</v>
+      </c>
+      <c r="O5" s="9">
+        <v>1</v>
+      </c>
+      <c r="P5" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="14">
+        <v>0</v>
+      </c>
+      <c r="R5" s="28">
+        <f>MAX(E5:E25,N5:N25)*1.05</f>
+        <v>35.700000000000003</v>
+      </c>
+      <c r="S5" s="28">
+        <f>B12</f>
+        <v>-25.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="9">
+        <v>-10</v>
+      </c>
+      <c r="E6" s="9">
+        <v>25</v>
+      </c>
+      <c r="F6" s="9">
+        <v>1</v>
+      </c>
+      <c r="G6" s="9">
+        <v>1</v>
+      </c>
+      <c r="H6" s="9">
+        <v>1</v>
+      </c>
+      <c r="I6" s="9">
+        <v>500</v>
+      </c>
+      <c r="J6" s="9">
+        <v>100</v>
+      </c>
+      <c r="K6" s="14">
+        <v>120</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="M6" s="9">
+        <v>10</v>
+      </c>
+      <c r="N6" s="9">
+        <v>34</v>
+      </c>
+      <c r="O6" s="9">
+        <v>1</v>
+      </c>
+      <c r="P6" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="14">
+        <v>0</v>
+      </c>
+      <c r="R6" s="28">
+        <v>0</v>
+      </c>
+      <c r="S6" s="28">
+        <f>B12</f>
+        <v>-25.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="18">
+        <v>60</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="8">
+        <v>-10</v>
+      </c>
+      <c r="E7" s="8">
+        <v>30</v>
+      </c>
+      <c r="F7" s="8">
+        <v>1</v>
+      </c>
+      <c r="G7" s="8">
+        <v>1</v>
+      </c>
+      <c r="H7" s="8">
+        <v>1</v>
+      </c>
+      <c r="I7" s="8">
+        <v>500</v>
+      </c>
+      <c r="J7" s="8">
+        <v>100</v>
+      </c>
+      <c r="K7" s="15">
+        <v>240</v>
+      </c>
+      <c r="L7" s="9"/>
+      <c r="R7" s="28"/>
+      <c r="S7" s="28">
+        <f>B13</f>
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="A8" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="18">
+        <v>100</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="9">
+        <v>10</v>
+      </c>
+      <c r="E8" s="9">
+        <v>20</v>
+      </c>
+      <c r="F8" s="9">
+        <v>1</v>
+      </c>
+      <c r="G8" s="9">
+        <v>1</v>
+      </c>
+      <c r="H8" s="9">
+        <v>1</v>
+      </c>
+      <c r="I8" s="9">
+        <v>500</v>
+      </c>
+      <c r="J8" s="9">
+        <v>100</v>
+      </c>
+      <c r="K8" s="14">
+        <v>0</v>
+      </c>
+      <c r="L8" s="9"/>
+      <c r="R8" s="28"/>
+      <c r="S8" s="28">
+        <f>B13</f>
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="A9" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="17">
+        <v>50</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="9">
+        <v>10</v>
+      </c>
+      <c r="E9" s="9">
+        <v>25</v>
+      </c>
+      <c r="F9" s="9">
+        <v>1</v>
+      </c>
+      <c r="G9" s="9">
+        <v>1</v>
+      </c>
+      <c r="H9" s="9">
+        <v>1</v>
+      </c>
+      <c r="I9" s="9">
+        <v>500</v>
+      </c>
+      <c r="J9" s="9">
+        <v>100</v>
+      </c>
+      <c r="K9" s="14">
+        <v>120</v>
+      </c>
+      <c r="L9" s="9"/>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="A10" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="17">
+        <v>1</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="8">
+        <v>10</v>
+      </c>
+      <c r="E10" s="8">
+        <v>30</v>
+      </c>
+      <c r="F10" s="8">
+        <v>1</v>
+      </c>
+      <c r="G10" s="8">
+        <v>1</v>
+      </c>
+      <c r="H10" s="8">
+        <v>1</v>
+      </c>
+      <c r="I10" s="8">
+        <v>500</v>
+      </c>
+      <c r="J10" s="8">
+        <v>100</v>
+      </c>
+      <c r="K10" s="15">
+        <v>240</v>
+      </c>
+      <c r="L10" s="9"/>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="A11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="18">
+        <v>3</v>
+      </c>
+      <c r="L11" s="9"/>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="A12" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="17">
+        <v>-25.5</v>
+      </c>
+      <c r="L12" s="9"/>
+    </row>
+    <row r="13" spans="1:19" ht="13.5" thickBot="1">
+      <c r="A13" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="20">
+        <v>25.5</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="1:19" ht="12.75" customHeight="1">
+      <c r="A14" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="37"/>
+      <c r="L14" s="9"/>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" s="38"/>
+      <c r="B15" s="39"/>
+      <c r="L15" s="9"/>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="C16" s="12"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="9"/>
+    </row>
+    <row r="17" spans="3:12">
+      <c r="L17" s="9"/>
+    </row>
+    <row r="18" spans="3:12">
+      <c r="L18" s="9"/>
+    </row>
+    <row r="19" spans="3:12">
+      <c r="C19" s="12"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="9"/>
+    </row>
+    <row r="22" spans="3:12">
+      <c r="C22" s="12"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="15"/>
+    </row>
+    <row r="25" spans="3:12">
+      <c r="C25" s="12"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:K3"/>
+    <mergeCell ref="L3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="A14:B15"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="0.75" header="0.5" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <headerFooter>
+    <oddHeader xml:space="preserve">&amp;L&amp;"-,Regular"&amp;9Draft&amp;C&amp;"Times New Roman,Bold"&amp;11 </oddHeader>
+    <oddFooter>&amp;L&amp;K4D4D4DG&amp;8RADIENT&amp;"Cambria,Regular"&amp;6
+&amp;"-,Regular"&amp;K4D4D4D
+&amp;Z&amp;F\&amp;A&amp;R&amp;"-,Regular"&amp;9Page &amp;P of &amp;N</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:S25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="35.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="21" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" style="11" customWidth="1"/>
+    <col min="4" max="10" width="10.42578125" style="9" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" style="14" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" style="6" customWidth="1"/>
+    <col min="13" max="16" width="10.42578125" style="9" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" style="14" customWidth="1"/>
+    <col min="18" max="18" width="22.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.85546875" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="25" customFormat="1" ht="15">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:19" s="26" customFormat="1">
+      <c r="A2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+    </row>
+    <row r="3" spans="1:19" ht="15.75">
+      <c r="A3" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="35"/>
+      <c r="C3" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="32"/>
+      <c r="R3" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="S3" s="33"/>
+    </row>
+    <row r="4" spans="1:19" ht="38.25">
+      <c r="A4" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q4" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="R4" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="S4" s="27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="9">
+        <v>-5</v>
+      </c>
+      <c r="E5" s="9">
+        <v>23</v>
+      </c>
+      <c r="F5" s="9">
+        <v>1</v>
+      </c>
+      <c r="G5" s="9">
+        <v>1</v>
+      </c>
+      <c r="H5" s="9">
+        <f>F5*G5</f>
+        <v>1</v>
+      </c>
+      <c r="I5" s="9">
+        <v>500</v>
+      </c>
+      <c r="J5" s="9">
+        <v>100</v>
+      </c>
+      <c r="K5" s="14">
+        <v>0</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="M5" s="9">
+        <v>3</v>
+      </c>
+      <c r="N5" s="9">
+        <v>34</v>
+      </c>
+      <c r="O5" s="9">
+        <v>1</v>
+      </c>
+      <c r="P5" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="14">
+        <v>0</v>
+      </c>
+      <c r="R5" s="28">
+        <f>MAX(E5:E25,N5:N25)*1.05</f>
+        <v>35.700000000000003</v>
+      </c>
+      <c r="S5" s="28">
+        <f>B12</f>
+        <v>-25.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0</v>
+      </c>
+      <c r="E6" s="9">
+        <v>23</v>
+      </c>
+      <c r="F6" s="9">
+        <v>1</v>
+      </c>
+      <c r="G6" s="9">
+        <v>1</v>
+      </c>
+      <c r="H6" s="9">
+        <v>1</v>
+      </c>
+      <c r="I6" s="9">
+        <v>500</v>
+      </c>
+      <c r="J6" s="9">
+        <v>100</v>
+      </c>
+      <c r="K6" s="14">
+        <v>120</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="M6" s="9">
+        <v>-3</v>
+      </c>
+      <c r="N6" s="9">
+        <v>34</v>
+      </c>
+      <c r="O6" s="9">
+        <v>1</v>
+      </c>
+      <c r="P6" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="14">
+        <v>0</v>
+      </c>
+      <c r="R6" s="28">
+        <v>0</v>
+      </c>
+      <c r="S6" s="28">
+        <f>B12</f>
+        <v>-25.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="18">
+        <v>60</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="8">
+        <v>5</v>
+      </c>
+      <c r="E7" s="8">
+        <v>23</v>
+      </c>
+      <c r="F7" s="8">
+        <v>1</v>
+      </c>
+      <c r="G7" s="8">
+        <v>1</v>
+      </c>
+      <c r="H7" s="8">
+        <v>1</v>
+      </c>
+      <c r="I7" s="8">
+        <v>500</v>
+      </c>
+      <c r="J7" s="8">
+        <v>100</v>
+      </c>
+      <c r="K7" s="15">
+        <v>240</v>
+      </c>
+      <c r="L7" s="9"/>
+      <c r="R7" s="28"/>
+      <c r="S7" s="28">
+        <f>B13</f>
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="A8" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="18">
+        <v>100</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="9">
+        <v>-5</v>
+      </c>
+      <c r="E8" s="9">
+        <v>28</v>
+      </c>
+      <c r="F8" s="9">
+        <v>1</v>
+      </c>
+      <c r="G8" s="9">
+        <v>1</v>
+      </c>
+      <c r="H8" s="9">
+        <v>1</v>
+      </c>
+      <c r="I8" s="9">
+        <v>500</v>
+      </c>
+      <c r="J8" s="9">
+        <v>100</v>
+      </c>
+      <c r="K8" s="14">
+        <v>0</v>
+      </c>
+      <c r="L8" s="9"/>
+      <c r="R8" s="28"/>
+      <c r="S8" s="28">
+        <f>B13</f>
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="A9" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="17">
+        <v>50</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0</v>
+      </c>
+      <c r="E9" s="9">
+        <v>28</v>
+      </c>
+      <c r="F9" s="9">
+        <v>1</v>
+      </c>
+      <c r="G9" s="9">
+        <v>1</v>
+      </c>
+      <c r="H9" s="9">
+        <v>1</v>
+      </c>
+      <c r="I9" s="9">
+        <v>500</v>
+      </c>
+      <c r="J9" s="9">
+        <v>100</v>
+      </c>
+      <c r="K9" s="14">
+        <v>120</v>
+      </c>
+      <c r="L9" s="9"/>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="A10" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="17">
+        <v>1</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="8">
+        <v>5</v>
+      </c>
+      <c r="E10" s="8">
+        <v>28</v>
+      </c>
+      <c r="F10" s="8">
+        <v>1</v>
+      </c>
+      <c r="G10" s="8">
+        <v>1</v>
+      </c>
+      <c r="H10" s="8">
+        <v>1</v>
+      </c>
+      <c r="I10" s="8">
+        <v>500</v>
+      </c>
+      <c r="J10" s="8">
+        <v>100</v>
+      </c>
+      <c r="K10" s="15">
+        <v>240</v>
+      </c>
+      <c r="L10" s="9"/>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="A11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="18">
+        <v>3</v>
+      </c>
+      <c r="L11" s="9"/>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="A12" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="17">
+        <v>-25.5</v>
+      </c>
+      <c r="L12" s="9"/>
+    </row>
+    <row r="13" spans="1:19" ht="13.5" thickBot="1">
+      <c r="A13" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="20">
+        <v>25.5</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="1:19" ht="12.75" customHeight="1">
+      <c r="A14" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="37"/>
+      <c r="L14" s="9"/>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="A15" s="38"/>
+      <c r="B15" s="39"/>
+      <c r="L15" s="9"/>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="C16" s="12"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="9"/>
+    </row>
+    <row r="17" spans="3:12">
+      <c r="L17" s="9"/>
+    </row>
+    <row r="18" spans="3:12">
+      <c r="L18" s="9"/>
+    </row>
+    <row r="19" spans="3:12">
+      <c r="C19" s="12"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="9"/>
+    </row>
+    <row r="22" spans="3:12">
+      <c r="C22" s="12"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="15"/>
+    </row>
+    <row r="25" spans="3:12">
+      <c r="C25" s="12"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:K3"/>
+    <mergeCell ref="L3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="A14:B15"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="0.75" header="0.5" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <headerFooter>
+    <oddHeader xml:space="preserve">&amp;L&amp;"-,Regular"&amp;9Draft&amp;C&amp;"Times New Roman,Bold"&amp;11 </oddHeader>
+    <oddFooter>&amp;L&amp;K4D4D4DG&amp;8RADIENT&amp;"Cambria,Regular"&amp;6
+&amp;"-,Regular"&amp;K4D4D4D
+&amp;Z&amp;F\&amp;A&amp;R&amp;"-,Regular"&amp;9Page &amp;P of &amp;N</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implement treatement of underground conductors, refine DAT comparison with rounding
</commit_message>
<xml_diff>
--- a/XC-template.xlsx
+++ b/XC-template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr backupFile="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="19140" windowHeight="14475" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="19140" windowHeight="14475" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="xc1" sheetId="1" r:id="rId1"/>
@@ -12,8 +12,9 @@
     <sheet name="xc3" sheetId="3" r:id="rId3"/>
     <sheet name="xc4" sheetId="4" r:id="rId4"/>
     <sheet name="xc5" sheetId="5" r:id="rId5"/>
+    <sheet name="xc_und" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="60">
   <si>
     <t>FIELDS Template</t>
   </si>
@@ -148,19 +149,61 @@
     <t>Main Title</t>
   </si>
   <si>
-    <t>Cross Section 2</t>
+    <t>Conductor Diameter</t>
   </si>
   <si>
-    <t>Cross Section 1</t>
+    <t>Bundle Diameter</t>
   </si>
   <si>
-    <t>Cross Section 3</t>
+    <t>Phase-Phase (kV)</t>
   </si>
   <si>
-    <t>Cross Section 4</t>
+    <t>Phase Current (Amp)</t>
   </si>
   <si>
-    <t>Cross Section 5</t>
+    <t>3b</t>
+  </si>
+  <si>
+    <t>3g</t>
+  </si>
+  <si>
+    <t>Post-Project, Mile 7.65 to Mile 7.88</t>
+  </si>
+  <si>
+    <t>3c</t>
+  </si>
+  <si>
+    <t>3a</t>
+  </si>
+  <si>
+    <t>Maximum Horizontal Distance From Reference (ft)</t>
+  </si>
+  <si>
+    <t>nc</t>
+  </si>
+  <si>
+    <t>nb</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>xc1</t>
+  </si>
+  <si>
+    <t>xc2</t>
+  </si>
+  <si>
+    <t>xc3</t>
+  </si>
+  <si>
+    <t>xc4</t>
+  </si>
+  <si>
+    <t>xc5</t>
+  </si>
+  <si>
+    <t>xc_und</t>
   </si>
 </sst>
 </file>
@@ -243,7 +286,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -419,13 +462,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -492,6 +557,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -521,6 +598,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -615,7 +695,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>Cross Section 1</c:v>
+              <c:v>xc1</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -840,23 +920,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="71157248"/>
-        <c:axId val="71158784"/>
+        <c:axId val="67823488"/>
+        <c:axId val="67825024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="71157248"/>
+        <c:axId val="67823488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71158784"/>
+        <c:crossAx val="67825024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71158784"/>
+        <c:axId val="67825024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -864,7 +944,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71157248"/>
+        <c:crossAx val="67823488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -878,7 +958,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000222" l="0.70000000000000118" r="0.70000000000000118" t="0.75000000000000222" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000151" r="0.70000000000000151" t="0.75000000000000255" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -895,7 +975,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>Cross Section 2</c:v>
+              <c:v>xc2</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -1120,23 +1200,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="118545408"/>
-        <c:axId val="120738560"/>
+        <c:axId val="76478720"/>
+        <c:axId val="82465152"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="118545408"/>
+        <c:axId val="76478720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120738560"/>
+        <c:crossAx val="82465152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="120738560"/>
+        <c:axId val="82465152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1144,7 +1224,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="118545408"/>
+        <c:crossAx val="76478720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1158,7 +1238,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000222" l="0.70000000000000118" r="0.70000000000000118" t="0.75000000000000222" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000151" r="0.70000000000000151" t="0.75000000000000255" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1175,7 +1255,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>Cross Section 3</c:v>
+              <c:v>xc3</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -1400,23 +1480,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="120785920"/>
-        <c:axId val="120787712"/>
+        <c:axId val="74150272"/>
+        <c:axId val="74151808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="120785920"/>
+        <c:axId val="74150272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120787712"/>
+        <c:crossAx val="74151808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="120787712"/>
+        <c:axId val="74151808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1424,7 +1504,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="120785920"/>
+        <c:crossAx val="74150272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1438,7 +1518,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000244" l="0.7000000000000014" r="0.7000000000000014" t="0.75000000000000244" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000278" l="0.70000000000000162" r="0.70000000000000162" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1455,7 +1535,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>Cross Section 4</c:v>
+              <c:v>xc4</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -1680,23 +1760,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="129738624"/>
-        <c:axId val="129740160"/>
+        <c:axId val="74178944"/>
+        <c:axId val="74180480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="129738624"/>
+        <c:axId val="74178944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="129740160"/>
+        <c:crossAx val="74180480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="129740160"/>
+        <c:axId val="74180480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1704,7 +1784,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="129738624"/>
+        <c:crossAx val="74178944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1718,7 +1798,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000266" l="0.70000000000000162" r="0.70000000000000162" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000003" l="0.70000000000000162" r="0.70000000000000162" t="0.750000000000003" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1735,7 +1815,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>Cross Section 5</c:v>
+              <c:v>xc5</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -1960,23 +2040,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="130069248"/>
-        <c:axId val="130070784"/>
+        <c:axId val="74629504"/>
+        <c:axId val="74631040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="130069248"/>
+        <c:axId val="74629504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130070784"/>
+        <c:crossAx val="74631040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="130070784"/>
+        <c:axId val="74631040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1984,7 +2064,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="130069248"/>
+        <c:crossAx val="74629504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1998,7 +2078,304 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000289" l="0.70000000000000162" r="0.70000000000000162" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000322" l="0.70000000000000162" r="0.70000000000000162" t="0.75000000000000322" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:strRef>
+          <c:f>xc_und!$B$5</c:f>
+          <c:strCache>
+            <c:ptCount val="1"/>
+            <c:pt idx="0">
+              <c:v>xc_und</c:v>
+            </c:pt>
+          </c:strCache>
+        </c:strRef>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Conductor Coordinates</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>xc_und!$D$5:$D$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>-8.42</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-11.67</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-8.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.42</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.67</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.75</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18.670000000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>19.329999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>xc_und!$E$5:$E$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>44.17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32.17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.170000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44.17</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32.17</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.170000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-5</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Ground Wire Coordinates</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="x"/>
+            <c:size val="7"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>xc_und!$M$5:$M$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>-6.33</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.33</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>xc_und!$N$5:$N$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>55.17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>55.17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Right ROW Edge</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="accent4">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>xc_und!$S$7:$S$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>xc_und!$R$5:$R$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>57.928500000000007</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Left ROW Edge</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:prstDash val="dash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>xc_und!$S$5:$S$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>-50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>xc_und!$R$5:$R$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>57.928500000000007</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+        </c:ser>
+        <c:axId val="74682752"/>
+        <c:axId val="74684288"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="74682752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="74684288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="74684288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="74682752"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000366" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000366" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2158,6 +2535,41 @@
       <xdr:colOff>666750</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2467,7 +2879,7 @@
   <dimension ref="A1:S25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -2526,33 +2938,33 @@
       <c r="P2" s="5"/>
     </row>
     <row r="3" spans="1:19" ht="15.75">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="30" t="s">
+      <c r="B3" s="41"/>
+      <c r="C3" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="30" t="s">
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="31"/>
-      <c r="N3" s="31"/>
-      <c r="O3" s="31"/>
-      <c r="P3" s="31"/>
-      <c r="Q3" s="32"/>
-      <c r="R3" s="33" t="s">
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="S3" s="33"/>
+      <c r="S3" s="39"/>
     </row>
     <row r="4" spans="1:19" ht="38.25">
       <c r="A4" s="23" t="s">
@@ -2618,7 +3030,7 @@
         <v>26</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>31</v>
@@ -2926,15 +3338,15 @@
       <c r="L13" s="9"/>
     </row>
     <row r="14" spans="1:19" ht="12.75" customHeight="1">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="37"/>
+      <c r="B14" s="43"/>
       <c r="L14" s="9"/>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="38"/>
-      <c r="B15" s="39"/>
+      <c r="A15" s="44"/>
+      <c r="B15" s="45"/>
       <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:19">
@@ -3021,7 +3433,7 @@
   <dimension ref="A1:S25"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -3080,33 +3492,33 @@
       <c r="P2" s="5"/>
     </row>
     <row r="3" spans="1:19" ht="15.75">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="30" t="s">
+      <c r="B3" s="41"/>
+      <c r="C3" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="30" t="s">
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="31"/>
-      <c r="N3" s="31"/>
-      <c r="O3" s="31"/>
-      <c r="P3" s="31"/>
-      <c r="Q3" s="32"/>
-      <c r="R3" s="33" t="s">
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="S3" s="33"/>
+      <c r="S3" s="39"/>
     </row>
     <row r="4" spans="1:19" ht="38.25">
       <c r="A4" s="23" t="s">
@@ -3172,7 +3584,7 @@
         <v>40</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>31</v>
@@ -3480,15 +3892,15 @@
       <c r="L13" s="9"/>
     </row>
     <row r="14" spans="1:19" ht="12.75" customHeight="1">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="37"/>
+      <c r="B14" s="43"/>
       <c r="L14" s="9"/>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="38"/>
-      <c r="B15" s="39"/>
+      <c r="A15" s="44"/>
+      <c r="B15" s="45"/>
       <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:19">
@@ -3574,7 +3986,7 @@
   <dimension ref="A1:S25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -3633,33 +4045,33 @@
       <c r="P2" s="5"/>
     </row>
     <row r="3" spans="1:19" ht="15.75">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="30" t="s">
+      <c r="B3" s="41"/>
+      <c r="C3" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="30" t="s">
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="31"/>
-      <c r="N3" s="31"/>
-      <c r="O3" s="31"/>
-      <c r="P3" s="31"/>
-      <c r="Q3" s="32"/>
-      <c r="R3" s="33" t="s">
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="S3" s="33"/>
+      <c r="S3" s="39"/>
     </row>
     <row r="4" spans="1:19" ht="38.25">
       <c r="A4" s="23" t="s">
@@ -3725,7 +4137,7 @@
         <v>40</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>31</v>
@@ -4033,15 +4445,15 @@
       <c r="L13" s="9"/>
     </row>
     <row r="14" spans="1:19" ht="12.75" customHeight="1">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="37"/>
+      <c r="B14" s="43"/>
       <c r="L14" s="9"/>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="38"/>
-      <c r="B15" s="39"/>
+      <c r="A15" s="44"/>
+      <c r="B15" s="45"/>
       <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:19">
@@ -4121,8 +4533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -4181,33 +4593,33 @@
       <c r="P2" s="5"/>
     </row>
     <row r="3" spans="1:19" ht="15.75">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="30" t="s">
+      <c r="B3" s="41"/>
+      <c r="C3" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="30" t="s">
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="31"/>
-      <c r="N3" s="31"/>
-      <c r="O3" s="31"/>
-      <c r="P3" s="31"/>
-      <c r="Q3" s="32"/>
-      <c r="R3" s="33" t="s">
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="S3" s="33"/>
+      <c r="S3" s="39"/>
     </row>
     <row r="4" spans="1:19" ht="38.25">
       <c r="A4" s="23" t="s">
@@ -4273,7 +4685,7 @@
         <v>40</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>31</v>
@@ -4581,15 +4993,15 @@
       <c r="L13" s="9"/>
     </row>
     <row r="14" spans="1:19" ht="12.75" customHeight="1">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="37"/>
+      <c r="B14" s="43"/>
       <c r="L14" s="9"/>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="38"/>
-      <c r="B15" s="39"/>
+      <c r="A15" s="44"/>
+      <c r="B15" s="45"/>
       <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:19">
@@ -4669,8 +5081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -4729,33 +5141,33 @@
       <c r="P2" s="5"/>
     </row>
     <row r="3" spans="1:19" ht="15.75">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="30" t="s">
+      <c r="B3" s="41"/>
+      <c r="C3" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="30" t="s">
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="31"/>
-      <c r="N3" s="31"/>
-      <c r="O3" s="31"/>
-      <c r="P3" s="31"/>
-      <c r="Q3" s="32"/>
-      <c r="R3" s="33" t="s">
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="38"/>
+      <c r="R3" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="S3" s="33"/>
+      <c r="S3" s="39"/>
     </row>
     <row r="4" spans="1:19" ht="38.25">
       <c r="A4" s="23" t="s">
@@ -4821,7 +5233,7 @@
         <v>40</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>31</v>
@@ -5129,15 +5541,15 @@
       <c r="L13" s="9"/>
     </row>
     <row r="14" spans="1:19" ht="12.75" customHeight="1">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="37"/>
+      <c r="B14" s="43"/>
       <c r="L14" s="9"/>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="38"/>
-      <c r="B15" s="39"/>
+      <c r="A15" s="44"/>
+      <c r="B15" s="45"/>
       <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:19">
@@ -5211,4 +5623,582 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:S25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="41.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" style="11" customWidth="1"/>
+    <col min="4" max="10" width="10.5703125" style="9" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" style="14" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" style="6" customWidth="1"/>
+    <col min="13" max="16" width="10.5703125" style="9" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" style="34" customWidth="1"/>
+    <col min="18" max="18" width="22.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="15">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" s="5" customFormat="1">
+      <c r="A2" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" s="30" customFormat="1" ht="15.75">
+      <c r="A3" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="41"/>
+      <c r="C3" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="37"/>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="37"/>
+      <c r="R3" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="S3" s="46"/>
+    </row>
+    <row r="4" spans="1:19" ht="38.25">
+      <c r="A4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q4" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="R4" s="33" t="s">
+        <v>20</v>
+      </c>
+      <c r="S4" s="33" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19">
+      <c r="A5" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="9">
+        <v>-8.42</v>
+      </c>
+      <c r="E5" s="9">
+        <v>44.17</v>
+      </c>
+      <c r="F5" s="9">
+        <v>1</v>
+      </c>
+      <c r="G5" s="9">
+        <v>1.29</v>
+      </c>
+      <c r="H5" s="9">
+        <v>1.29</v>
+      </c>
+      <c r="I5" s="9">
+        <v>1150</v>
+      </c>
+      <c r="J5" s="9">
+        <v>1664</v>
+      </c>
+      <c r="K5" s="14">
+        <v>120</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="M5" s="9">
+        <v>-6.33</v>
+      </c>
+      <c r="N5" s="9">
+        <v>55.17</v>
+      </c>
+      <c r="O5" s="9">
+        <v>1</v>
+      </c>
+      <c r="P5" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="34">
+        <v>0</v>
+      </c>
+      <c r="R5" s="35">
+        <f>MAX(E5:E25,N5:N25)*1.05</f>
+        <v>57.928500000000007</v>
+      </c>
+      <c r="S5" s="35">
+        <f>B12</f>
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19">
+      <c r="A6" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="9">
+        <v>-11.67</v>
+      </c>
+      <c r="E6" s="9">
+        <v>32.17</v>
+      </c>
+      <c r="F6" s="9">
+        <v>1</v>
+      </c>
+      <c r="G6" s="9">
+        <v>1.29</v>
+      </c>
+      <c r="H6" s="9">
+        <v>1.29</v>
+      </c>
+      <c r="I6" s="9">
+        <v>1150</v>
+      </c>
+      <c r="J6" s="9">
+        <v>1664</v>
+      </c>
+      <c r="K6" s="14">
+        <v>240</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="M6" s="9">
+        <v>4.33</v>
+      </c>
+      <c r="N6" s="9">
+        <v>55.17</v>
+      </c>
+      <c r="O6" s="9">
+        <v>1</v>
+      </c>
+      <c r="P6" s="9">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="34">
+        <v>0</v>
+      </c>
+      <c r="R6" s="35">
+        <v>0</v>
+      </c>
+      <c r="S6" s="35">
+        <f>B12</f>
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19">
+      <c r="A7" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="18">
+        <v>60</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D7" s="8">
+        <v>-8.75</v>
+      </c>
+      <c r="E7" s="8">
+        <v>20.170000000000002</v>
+      </c>
+      <c r="F7" s="8">
+        <v>1</v>
+      </c>
+      <c r="G7" s="8">
+        <v>1.29</v>
+      </c>
+      <c r="H7" s="8">
+        <v>1.29</v>
+      </c>
+      <c r="I7" s="8">
+        <v>1150</v>
+      </c>
+      <c r="J7" s="8">
+        <v>1664</v>
+      </c>
+      <c r="K7" s="15">
+        <v>0</v>
+      </c>
+      <c r="L7" s="9"/>
+      <c r="R7" s="35"/>
+      <c r="S7" s="35">
+        <f>B13</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="A8" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="18">
+        <v>100</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="9">
+        <v>6.42</v>
+      </c>
+      <c r="E8" s="9">
+        <v>44.17</v>
+      </c>
+      <c r="F8" s="9">
+        <v>1</v>
+      </c>
+      <c r="G8" s="9">
+        <v>1.29</v>
+      </c>
+      <c r="H8" s="9">
+        <v>1.29</v>
+      </c>
+      <c r="I8" s="9">
+        <v>1150</v>
+      </c>
+      <c r="J8" s="9">
+        <v>1664</v>
+      </c>
+      <c r="K8" s="14">
+        <v>240</v>
+      </c>
+      <c r="L8" s="9"/>
+      <c r="R8" s="35"/>
+      <c r="S8" s="35">
+        <f>B13</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19">
+      <c r="A9" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="17">
+        <v>150</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="9">
+        <v>9.67</v>
+      </c>
+      <c r="E9" s="9">
+        <v>32.17</v>
+      </c>
+      <c r="F9" s="9">
+        <v>1</v>
+      </c>
+      <c r="G9" s="9">
+        <v>1.29</v>
+      </c>
+      <c r="H9" s="9">
+        <v>1.29</v>
+      </c>
+      <c r="I9" s="9">
+        <v>1150</v>
+      </c>
+      <c r="J9" s="9">
+        <v>1664</v>
+      </c>
+      <c r="K9" s="14">
+        <v>0</v>
+      </c>
+      <c r="L9" s="9"/>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="A10" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="17">
+        <v>1</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="8">
+        <v>6.75</v>
+      </c>
+      <c r="E10" s="8">
+        <v>20.170000000000002</v>
+      </c>
+      <c r="F10" s="8">
+        <v>1</v>
+      </c>
+      <c r="G10" s="8">
+        <v>1.29</v>
+      </c>
+      <c r="H10" s="8">
+        <v>1.29</v>
+      </c>
+      <c r="I10" s="8">
+        <v>1150</v>
+      </c>
+      <c r="J10" s="8">
+        <v>1664</v>
+      </c>
+      <c r="K10" s="15">
+        <v>120</v>
+      </c>
+      <c r="L10" s="9"/>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="A11" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="18">
+        <v>3</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="9">
+        <v>18.670000000000002</v>
+      </c>
+      <c r="E11" s="9">
+        <v>-5</v>
+      </c>
+      <c r="F11" s="9">
+        <v>1</v>
+      </c>
+      <c r="G11" s="9">
+        <v>0.68</v>
+      </c>
+      <c r="H11" s="9">
+        <v>0.68</v>
+      </c>
+      <c r="I11" s="9">
+        <v>3450</v>
+      </c>
+      <c r="J11" s="9">
+        <v>764</v>
+      </c>
+      <c r="K11" s="14">
+        <v>240</v>
+      </c>
+      <c r="L11" s="9"/>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="A12" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="17">
+        <v>-50</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="9">
+        <v>19</v>
+      </c>
+      <c r="E12" s="9">
+        <v>-5</v>
+      </c>
+      <c r="F12" s="9">
+        <v>1</v>
+      </c>
+      <c r="G12" s="9">
+        <v>0.68</v>
+      </c>
+      <c r="H12" s="9">
+        <v>0.68</v>
+      </c>
+      <c r="I12" s="9">
+        <v>3450</v>
+      </c>
+      <c r="J12" s="9">
+        <v>764</v>
+      </c>
+      <c r="K12" s="14">
+        <v>120</v>
+      </c>
+      <c r="L12" s="9"/>
+    </row>
+    <row r="13" spans="1:19" ht="13.5" thickBot="1">
+      <c r="A13" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="20">
+        <v>50</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="8">
+        <v>19.329999999999998</v>
+      </c>
+      <c r="E13" s="8">
+        <v>-5</v>
+      </c>
+      <c r="F13" s="8">
+        <v>1</v>
+      </c>
+      <c r="G13" s="8">
+        <v>0.68</v>
+      </c>
+      <c r="H13" s="8">
+        <v>0.68</v>
+      </c>
+      <c r="I13" s="8">
+        <v>3450</v>
+      </c>
+      <c r="J13" s="8">
+        <v>764</v>
+      </c>
+      <c r="K13" s="15">
+        <v>0</v>
+      </c>
+      <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="L14" s="9"/>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="L15" s="9"/>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="C16" s="12"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="9"/>
+    </row>
+    <row r="17" spans="3:12">
+      <c r="L17" s="9"/>
+    </row>
+    <row r="18" spans="3:12">
+      <c r="L18" s="9"/>
+    </row>
+    <row r="19" spans="3:12">
+      <c r="C19" s="12"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="9"/>
+    </row>
+    <row r="22" spans="3:12">
+      <c r="C22" s="12"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="15"/>
+    </row>
+    <row r="25" spans="3:12">
+      <c r="C25" s="12"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:K3"/>
+    <mergeCell ref="L3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+  </mergeCells>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="0.75" header="0.5" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader xml:space="preserve">&amp;L&amp;"-,Regular"&amp;9Draft&amp;C&amp;"Times New Roman,Bold"&amp;11 </oddHeader>
+    <oddFooter>&amp;L&amp;K4D4D4DG&amp;8RADIENT&amp;"Cambria,Regular"&amp;6
+&amp;"-,Regular"&amp;K4D4D4D
+&amp;Z&amp;F\&amp;A&amp;R&amp;"-,Regular"&amp;9Page &amp;P of &amp;N</oddFooter>
+  </headerFooter>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Start tag & group functions
</commit_message>
<xml_diff>
--- a/XC-template.xlsx
+++ b/XC-template.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr backupFile="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25317"/>
+  <workbookPr backupFile="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="19140" windowHeight="14475" activeTab="4"/>
+    <workbookView xWindow="-80" yWindow="0" windowWidth="25380" windowHeight="16860" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="xc1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="xc5" sheetId="5" r:id="rId5"/>
     <sheet name="xc_und" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="61">
   <si>
     <t>FIELDS Template</t>
   </si>
@@ -205,12 +205,15 @@
   <si>
     <t>xc_und</t>
   </si>
+  <si>
+    <t>Group Tag</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -264,6 +267,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -465,30 +480,44 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -603,7 +632,21 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="17">
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal_TMPLTS" xfId="1"/>
@@ -686,7 +729,17 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -701,11 +754,14 @@
         </c:strRef>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -723,58 +779,59 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'xc1'!$D$5:$D$31</c:f>
+              <c:f>'xc1'!$D$5:$D$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>-10</c:v>
+                  <c:v>-10.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-5</c:v>
+                  <c:v>-5.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-5</c:v>
+                  <c:v>-5.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'xc1'!$E$5:$E$32</c:f>
+              <c:f>'xc1'!$E$5:$E$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22</c:v>
+                  <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28</c:v>
+                  <c:v>28.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22</c:v>
+                  <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>28</c:v>
+                  <c:v>28.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -793,34 +850,35 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'xc1'!$M$5:$M$12</c:f>
+              <c:f>'xc1'!$M$5:$M$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>-5</c:v>
+                  <c:v>-5.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'xc1'!$N$5:$N$12</c:f>
+              <c:f>'xc1'!$N$5:$N$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -866,11 +924,12 @@
                   <c:v>33.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -914,37 +973,52 @@
                   <c:v>33.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="71753088"/>
-        <c:axId val="71756032"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2133867032"/>
+        <c:axId val="2133863992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="71753088"/>
+        <c:axId val="2133867032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71756032"/>
+        <c:crossAx val="2133863992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="71756032"/>
+        <c:axId val="2133863992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71753088"/>
+        <c:crossAx val="2133867032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -952,13 +1026,15 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000266" l="0.70000000000000162" r="0.70000000000000162" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000003" l="0.700000000000002" r="0.700000000000002" t="0.750000000000003" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -966,7 +1042,17 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -981,11 +1067,14 @@
         </c:strRef>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1003,58 +1092,59 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'xc2'!$D$5:$D$31</c:f>
+              <c:f>'xc2'!$D$5:$D$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>-5</c:v>
+                  <c:v>-5.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-7</c:v>
+                  <c:v>-7.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-5</c:v>
+                  <c:v>-5.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'xc2'!$E$5:$E$32</c:f>
+              <c:f>'xc2'!$E$5:$E$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27</c:v>
+                  <c:v>27.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>32</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27</c:v>
+                  <c:v>27.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1073,34 +1163,35 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'xc2'!$M$5:$M$12</c:f>
+              <c:f>'xc2'!$M$5:$M$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>-2</c:v>
+                  <c:v>-2.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'xc2'!$N$5:$N$12</c:f>
+              <c:f>'xc2'!$N$5:$N$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>35.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>35</c:v>
+                  <c:v>35.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1146,11 +1237,12 @@
                   <c:v>36.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1194,37 +1286,52 @@
                   <c:v>36.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="135880064"/>
-        <c:axId val="146548224"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2136459384"/>
+        <c:axId val="2136462520"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="135880064"/>
+        <c:axId val="2136459384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="146548224"/>
+        <c:crossAx val="2136462520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="146548224"/>
+        <c:axId val="2136462520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="135880064"/>
+        <c:crossAx val="2136459384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1232,13 +1339,15 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000266" l="0.70000000000000162" r="0.70000000000000162" t="0.75000000000000266" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000003" l="0.700000000000002" r="0.700000000000002" t="0.750000000000003" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1246,7 +1355,17 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1261,11 +1380,14 @@
         </c:strRef>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1283,58 +1405,59 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'xc3'!$D$5:$D$31</c:f>
+              <c:f>'xc3'!$D$5:$D$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>-12</c:v>
+                  <c:v>-12.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-8</c:v>
+                  <c:v>-8.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-4</c:v>
+                  <c:v>-4.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'xc3'!$E$5:$E$32</c:f>
+              <c:f>'xc3'!$E$5:$E$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1353,34 +1476,35 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'xc3'!$M$5:$M$12</c:f>
+              <c:f>'xc3'!$M$5:$M$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>-10</c:v>
+                  <c:v>-10.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'xc3'!$N$5:$N$12</c:f>
+              <c:f>'xc3'!$N$5:$N$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>28</c:v>
+                  <c:v>28.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28</c:v>
+                  <c:v>28.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1423,14 +1547,15 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>29.400000000000002</c:v>
+                  <c:v>29.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1471,40 +1596,55 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>29.400000000000002</c:v>
+                  <c:v>29.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="72470912"/>
-        <c:axId val="72472448"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2136511048"/>
+        <c:axId val="2136514184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="72470912"/>
+        <c:axId val="2136511048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72472448"/>
+        <c:crossAx val="2136514184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="72472448"/>
+        <c:axId val="2136514184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72470912"/>
+        <c:crossAx val="2136511048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1512,13 +1652,15 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000289" l="0.70000000000000162" r="0.70000000000000162" t="0.75000000000000289" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000003" l="0.700000000000002" r="0.700000000000002" t="0.750000000000003" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1526,7 +1668,17 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1541,11 +1693,14 @@
         </c:strRef>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1563,58 +1718,59 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'xc4'!$D$5:$D$31</c:f>
+              <c:f>'xc4'!$D$5:$D$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>-10</c:v>
+                  <c:v>-10.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-10</c:v>
+                  <c:v>-10.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-10</c:v>
+                  <c:v>-10.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'xc4'!$E$5:$E$32</c:f>
+              <c:f>'xc4'!$E$5:$E$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>30.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30</c:v>
+                  <c:v>30.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1633,34 +1789,35 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'xc4'!$M$5:$M$12</c:f>
+              <c:f>'xc4'!$M$5:$M$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>-10</c:v>
+                  <c:v>-10.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>10.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'xc4'!$N$5:$N$12</c:f>
+              <c:f>'xc4'!$N$5:$N$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>34</c:v>
+                  <c:v>34.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34</c:v>
+                  <c:v>34.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1703,14 +1860,15 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>35.700000000000003</c:v>
+                  <c:v>35.7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1751,40 +1909,55 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>35.700000000000003</c:v>
+                  <c:v>35.7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="109461888"/>
-        <c:axId val="109463424"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2135498520"/>
+        <c:axId val="2135501656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="109461888"/>
+        <c:axId val="2135498520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109463424"/>
+        <c:crossAx val="2135501656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="109463424"/>
+        <c:axId val="2135501656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109461888"/>
+        <c:crossAx val="2135498520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1792,13 +1965,15 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000311" l="0.70000000000000162" r="0.70000000000000162" t="0.75000000000000311" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000003" l="0.700000000000002" r="0.700000000000002" t="0.750000000000003" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1806,7 +1981,17 @@
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1821,11 +2006,14 @@
         </c:strRef>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1843,58 +2031,59 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'xc5'!$D$5:$D$31</c:f>
+              <c:f>'xc5'!$D$5:$D$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
-                  <c:v>-5</c:v>
+                  <c:v>-5.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-5</c:v>
+                  <c:v>-5.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'xc5'!$E$5:$E$32</c:f>
+              <c:f>'xc5'!$E$5:$E$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23</c:v>
+                  <c:v>23.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>28</c:v>
+                  <c:v>28.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28</c:v>
+                  <c:v>28.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>28</c:v>
+                  <c:v>28.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1913,34 +2102,35 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'xc5'!$M$5:$M$12</c:f>
+              <c:f>'xc5'!$M$5:$M$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-3</c:v>
+                  <c:v>-3.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'xc5'!$N$5:$N$12</c:f>
+              <c:f>'xc5'!$N$5:$N$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>34</c:v>
+                  <c:v>34.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>34</c:v>
+                  <c:v>34.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1983,14 +2173,15 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>35.700000000000003</c:v>
+                  <c:v>35.7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -2031,40 +2222,55 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>35.700000000000003</c:v>
+                  <c:v>35.7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="109670784"/>
-        <c:axId val="109672320"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2135550456"/>
+        <c:axId val="2135553592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="109670784"/>
+        <c:axId val="2135550456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109672320"/>
+        <c:crossAx val="2135553592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="109672320"/>
+        <c:axId val="2135553592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109670784"/>
+        <c:crossAx val="2135550456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2072,13 +2278,15 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000333" l="0.70000000000000162" r="0.70000000000000162" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000003" l="0.700000000000002" r="0.700000000000002" t="0.750000000000003" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2086,7 +2294,17 @@
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2101,11 +2319,14 @@
         </c:strRef>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -2123,10 +2344,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>xc_und!$D$5:$D$31</c:f>
+              <c:f>xc_und!$D$5:$D$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="27"/>
+                <c:ptCount val="28"/>
                 <c:pt idx="0">
                   <c:v>-8.42</c:v>
                 </c:pt>
@@ -2146,23 +2367,23 @@
                   <c:v>6.75</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>18.670000000000002</c:v>
+                  <c:v>18.67</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>19</c:v>
+                  <c:v>19.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>19.329999999999998</c:v>
+                  <c:v>19.33</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>xc_und!$E$5:$E$32</c:f>
+              <c:f>xc_und!$E$5:$E$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
+                <c:ptCount val="29"/>
                 <c:pt idx="0">
                   <c:v>44.17</c:v>
                 </c:pt>
@@ -2170,7 +2391,7 @@
                   <c:v>32.17</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.170000000000002</c:v>
+                  <c:v>20.17</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>44.17</c:v>
@@ -2179,20 +2400,21 @@
                   <c:v>32.17</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20.170000000000002</c:v>
+                  <c:v>20.17</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-5</c:v>
+                  <c:v>-5.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-5</c:v>
+                  <c:v>-5.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-5</c:v>
+                  <c:v>-5.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2239,6 +2461,7 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2266,10 +2489,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>50</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50</c:v>
+                  <c:v>50.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2281,14 +2504,15 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>57.928500000000007</c:v>
+                  <c:v>57.9285</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -2314,10 +2538,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>-50</c:v>
+                  <c:v>-50.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-50</c:v>
+                  <c:v>-50.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2329,40 +2553,55 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>57.928500000000007</c:v>
+                  <c:v>57.9285</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="109764992"/>
-        <c:axId val="109766528"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2136569096"/>
+        <c:axId val="2136572232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="109764992"/>
+        <c:axId val="2136569096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109766528"/>
+        <c:crossAx val="2136572232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="109766528"/>
+        <c:axId val="2136572232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109764992"/>
+        <c:crossAx val="2136569096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2370,12 +2609,15 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000377" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000377" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000004" l="0.700000000000001" r="0.700000000000001" t="0.750000000000004" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2387,13 +2629,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2422,13 +2664,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2457,13 +2699,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2492,13 +2734,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2527,13 +2769,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2562,13 +2804,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2875,29 +3117,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="35.83203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="21" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="11" customWidth="1"/>
-    <col min="4" max="10" width="10.42578125" style="9" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" style="14" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" style="6" customWidth="1"/>
-    <col min="13" max="16" width="10.42578125" style="9" customWidth="1"/>
-    <col min="17" max="17" width="10.42578125" style="14" customWidth="1"/>
-    <col min="18" max="18" width="22.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.85546875" style="9"/>
+    <col min="3" max="3" width="10.5" style="11" customWidth="1"/>
+    <col min="4" max="10" width="10.5" style="9" customWidth="1"/>
+    <col min="11" max="11" width="10.5" style="14" customWidth="1"/>
+    <col min="12" max="12" width="10.5" style="6" customWidth="1"/>
+    <col min="13" max="16" width="10.5" style="9" customWidth="1"/>
+    <col min="17" max="17" width="10.5" style="14" customWidth="1"/>
+    <col min="18" max="18" width="22.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="25" customFormat="1" ht="15">
+    <row r="1" spans="1:19" s="25" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2937,7 +3179,7 @@
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
     </row>
-    <row r="3" spans="1:19" ht="15.75">
+    <row r="3" spans="1:19" ht="15">
       <c r="A3" s="40" t="s">
         <v>21</v>
       </c>
@@ -2966,7 +3208,7 @@
       </c>
       <c r="S3" s="39"/>
     </row>
-    <row r="4" spans="1:19" ht="38.25">
+    <row r="4" spans="1:19" ht="42">
       <c r="A4" s="23" t="s">
         <v>28</v>
       </c>
@@ -3079,20 +3321,20 @@
         <v>0</v>
       </c>
       <c r="R5" s="28">
-        <f>MAX(E5:E25,N5:N25)*1.05</f>
+        <f>MAX(E5:E26,N5:N26)*1.05</f>
         <v>33.6</v>
       </c>
       <c r="S5" s="28">
-        <f>B12</f>
+        <f>B13</f>
         <v>-25.5</v>
       </c>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>37</v>
+      <c r="A6" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="17">
+        <v>1</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>32</v>
@@ -3143,16 +3385,16 @@
         <v>0</v>
       </c>
       <c r="S6" s="28">
-        <f>B12</f>
+        <f>B13</f>
         <v>-25.5</v>
       </c>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="18">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>37</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>33</v>
@@ -3184,16 +3426,16 @@
       <c r="L7" s="9"/>
       <c r="R7" s="28"/>
       <c r="S7" s="28">
-        <f>B13</f>
+        <f>B14</f>
         <v>25.5</v>
       </c>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" s="18">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>34</v>
@@ -3225,16 +3467,16 @@
       <c r="L8" s="9"/>
       <c r="R8" s="28"/>
       <c r="S8" s="28">
-        <f>B13</f>
+        <f>B14</f>
         <v>25.5</v>
       </c>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="17">
-        <v>50</v>
+        <v>3</v>
+      </c>
+      <c r="B9" s="18">
+        <v>100</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>35</v>
@@ -3267,10 +3509,10 @@
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="16" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="B10" s="17">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>36</v>
@@ -3303,103 +3545,111 @@
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="18">
-        <v>3</v>
-      </c>
-      <c r="L11" s="9"/>
+        <v>4</v>
+      </c>
+      <c r="B11" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="18">
+        <v>3</v>
+      </c>
+      <c r="L12" s="9"/>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="A13" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="17">
+      <c r="B13" s="17">
         <v>-25.5</v>
       </c>
-      <c r="L12" s="9"/>
-    </row>
-    <row r="13" spans="1:19" ht="13.5" thickBot="1">
-      <c r="A13" s="19" t="s">
+      <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="1:19" ht="15" thickBot="1">
+      <c r="A14" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="20">
+      <c r="B14" s="20">
         <v>25.5</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="9"/>
-    </row>
-    <row r="14" spans="1:19" ht="12.75" customHeight="1">
-      <c r="A14" s="42" t="s">
+      <c r="C14" s="12"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="9"/>
+    </row>
+    <row r="15" spans="1:19" ht="12.75" customHeight="1">
+      <c r="A15" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="43"/>
-      <c r="L14" s="9"/>
-    </row>
-    <row r="15" spans="1:19">
-      <c r="A15" s="44"/>
-      <c r="B15" s="45"/>
+      <c r="B15" s="43"/>
       <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:19">
-      <c r="C16" s="12"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="15"/>
+      <c r="A16" s="44"/>
+      <c r="B16" s="45"/>
       <c r="L16" s="9"/>
     </row>
     <row r="17" spans="3:12">
+      <c r="C17" s="12"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="15"/>
       <c r="L17" s="9"/>
     </row>
     <row r="18" spans="3:12">
       <c r="L18" s="9"/>
     </row>
     <row r="19" spans="3:12">
-      <c r="C19" s="12"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="15"/>
       <c r="L19" s="9"/>
     </row>
-    <row r="22" spans="3:12">
-      <c r="C22" s="12"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="15"/>
-    </row>
-    <row r="25" spans="3:12">
-      <c r="C25" s="12"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="15"/>
+    <row r="20" spans="3:12">
+      <c r="C20" s="12"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="9"/>
+    </row>
+    <row r="23" spans="3:12">
+      <c r="C23" s="12"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="15"/>
+    </row>
+    <row r="26" spans="3:12">
+      <c r="C26" s="12"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3407,7 +3657,7 @@
     <mergeCell ref="L3:Q3"/>
     <mergeCell ref="R3:S3"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A14:B15"/>
+    <mergeCell ref="A15:B16"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -3429,29 +3679,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="35.83203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="21" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="11" customWidth="1"/>
-    <col min="4" max="10" width="10.42578125" style="9" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" style="14" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" style="6" customWidth="1"/>
-    <col min="13" max="16" width="10.42578125" style="9" customWidth="1"/>
-    <col min="17" max="17" width="10.42578125" style="14" customWidth="1"/>
-    <col min="18" max="18" width="22.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.85546875" style="9"/>
+    <col min="3" max="3" width="10.5" style="11" customWidth="1"/>
+    <col min="4" max="10" width="10.5" style="9" customWidth="1"/>
+    <col min="11" max="11" width="10.5" style="14" customWidth="1"/>
+    <col min="12" max="12" width="10.5" style="6" customWidth="1"/>
+    <col min="13" max="16" width="10.5" style="9" customWidth="1"/>
+    <col min="17" max="17" width="10.5" style="14" customWidth="1"/>
+    <col min="18" max="18" width="22.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="25" customFormat="1" ht="15">
+    <row r="1" spans="1:19" s="25" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -3491,7 +3741,7 @@
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
     </row>
-    <row r="3" spans="1:19" ht="15.75">
+    <row r="3" spans="1:19" ht="15">
       <c r="A3" s="40" t="s">
         <v>21</v>
       </c>
@@ -3520,7 +3770,7 @@
       </c>
       <c r="S3" s="39"/>
     </row>
-    <row r="4" spans="1:19" ht="38.25">
+    <row r="4" spans="1:19" ht="42">
       <c r="A4" s="23" t="s">
         <v>28</v>
       </c>
@@ -3633,20 +3883,20 @@
         <v>0</v>
       </c>
       <c r="R5" s="28">
-        <f>MAX(E5:E25,N5:N25)*1.05</f>
+        <f>MAX(E5:E26,N5:N26)*1.05</f>
         <v>36.75</v>
       </c>
       <c r="S5" s="28">
-        <f>B12</f>
+        <f>B13</f>
         <v>-25.5</v>
       </c>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>37</v>
+      <c r="A6" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="17">
+        <v>1</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>32</v>
@@ -3697,16 +3947,16 @@
         <v>0</v>
       </c>
       <c r="S6" s="28">
-        <f>B12</f>
+        <f>B13</f>
         <v>-25.5</v>
       </c>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="18">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>37</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>33</v>
@@ -3738,16 +3988,16 @@
       <c r="L7" s="9"/>
       <c r="R7" s="28"/>
       <c r="S7" s="28">
-        <f>B13</f>
+        <f>B14</f>
         <v>25.5</v>
       </c>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" s="18">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>34</v>
@@ -3779,16 +4029,16 @@
       <c r="L8" s="9"/>
       <c r="R8" s="28"/>
       <c r="S8" s="28">
-        <f>B13</f>
+        <f>B14</f>
         <v>25.5</v>
       </c>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="17">
-        <v>75</v>
+        <v>3</v>
+      </c>
+      <c r="B9" s="18">
+        <v>100</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>35</v>
@@ -3821,10 +4071,10 @@
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="16" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="B10" s="17">
-        <v>1</v>
+        <v>75</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>36</v>
@@ -3857,103 +4107,111 @@
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="18">
-        <v>3</v>
-      </c>
-      <c r="L11" s="9"/>
+        <v>4</v>
+      </c>
+      <c r="B11" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="18">
+        <v>3</v>
+      </c>
+      <c r="L12" s="9"/>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="A13" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="17">
+      <c r="B13" s="17">
         <v>-25.5</v>
       </c>
-      <c r="L12" s="9"/>
-    </row>
-    <row r="13" spans="1:19" ht="13.5" thickBot="1">
-      <c r="A13" s="19" t="s">
+      <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="1:19" ht="15" thickBot="1">
+      <c r="A14" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="20">
+      <c r="B14" s="20">
         <v>25.5</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="9"/>
-    </row>
-    <row r="14" spans="1:19" ht="12.75" customHeight="1">
-      <c r="A14" s="42" t="s">
+      <c r="C14" s="12"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="9"/>
+    </row>
+    <row r="15" spans="1:19" ht="12.75" customHeight="1">
+      <c r="A15" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="43"/>
-      <c r="L14" s="9"/>
-    </row>
-    <row r="15" spans="1:19">
-      <c r="A15" s="44"/>
-      <c r="B15" s="45"/>
+      <c r="B15" s="43"/>
       <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:19">
-      <c r="C16" s="12"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="15"/>
+      <c r="A16" s="44"/>
+      <c r="B16" s="45"/>
       <c r="L16" s="9"/>
     </row>
     <row r="17" spans="3:12">
+      <c r="C17" s="12"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="15"/>
       <c r="L17" s="9"/>
     </row>
     <row r="18" spans="3:12">
       <c r="L18" s="9"/>
     </row>
     <row r="19" spans="3:12">
-      <c r="C19" s="12"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="15"/>
       <c r="L19" s="9"/>
     </row>
-    <row r="22" spans="3:12">
-      <c r="C22" s="12"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="15"/>
-    </row>
-    <row r="25" spans="3:12">
-      <c r="C25" s="12"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="15"/>
+    <row r="20" spans="3:12">
+      <c r="C20" s="12"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="9"/>
+    </row>
+    <row r="23" spans="3:12">
+      <c r="C23" s="12"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="15"/>
+    </row>
+    <row r="26" spans="3:12">
+      <c r="C26" s="12"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3961,7 +4219,7 @@
     <mergeCell ref="C3:K3"/>
     <mergeCell ref="L3:Q3"/>
     <mergeCell ref="R3:S3"/>
-    <mergeCell ref="A14:B15"/>
+    <mergeCell ref="A15:B16"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="0.75" header="0.5" footer="0.3"/>
@@ -3982,29 +4240,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="35.83203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="21" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="11" customWidth="1"/>
-    <col min="4" max="10" width="10.42578125" style="9" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" style="14" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" style="6" customWidth="1"/>
-    <col min="13" max="16" width="10.42578125" style="9" customWidth="1"/>
-    <col min="17" max="17" width="10.42578125" style="14" customWidth="1"/>
-    <col min="18" max="18" width="22.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.85546875" style="9"/>
+    <col min="3" max="3" width="10.5" style="11" customWidth="1"/>
+    <col min="4" max="10" width="10.5" style="9" customWidth="1"/>
+    <col min="11" max="11" width="10.5" style="14" customWidth="1"/>
+    <col min="12" max="12" width="10.5" style="6" customWidth="1"/>
+    <col min="13" max="16" width="10.5" style="9" customWidth="1"/>
+    <col min="17" max="17" width="10.5" style="14" customWidth="1"/>
+    <col min="18" max="18" width="22.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="25" customFormat="1" ht="15">
+    <row r="1" spans="1:19" s="25" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -4044,7 +4302,7 @@
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
     </row>
-    <row r="3" spans="1:19" ht="15.75">
+    <row r="3" spans="1:19" ht="15">
       <c r="A3" s="40" t="s">
         <v>21</v>
       </c>
@@ -4073,7 +4331,7 @@
       </c>
       <c r="S3" s="39"/>
     </row>
-    <row r="4" spans="1:19" ht="38.25">
+    <row r="4" spans="1:19" ht="42">
       <c r="A4" s="23" t="s">
         <v>28</v>
       </c>
@@ -4186,20 +4444,20 @@
         <v>0</v>
       </c>
       <c r="R5" s="28">
-        <f>MAX(E5:E25,N5:N25)*1.05</f>
+        <f>MAX(E5:E26,N5:N26)*1.05</f>
         <v>29.400000000000002</v>
       </c>
       <c r="S5" s="28">
-        <f>B12</f>
+        <f>B13</f>
         <v>-25.5</v>
       </c>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>37</v>
+      <c r="A6" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="17">
+        <v>3</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>32</v>
@@ -4250,16 +4508,16 @@
         <v>0</v>
       </c>
       <c r="S6" s="28">
-        <f>B12</f>
+        <f>B13</f>
         <v>-25.5</v>
       </c>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="18">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>37</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>33</v>
@@ -4291,16 +4549,16 @@
       <c r="L7" s="9"/>
       <c r="R7" s="28"/>
       <c r="S7" s="28">
-        <f>B13</f>
+        <f>B14</f>
         <v>25.5</v>
       </c>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" s="18">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>34</v>
@@ -4332,16 +4590,16 @@
       <c r="L8" s="9"/>
       <c r="R8" s="28"/>
       <c r="S8" s="28">
-        <f>B13</f>
+        <f>B14</f>
         <v>25.5</v>
       </c>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="17">
-        <v>60</v>
+        <v>3</v>
+      </c>
+      <c r="B9" s="18">
+        <v>100</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>35</v>
@@ -4374,10 +4632,10 @@
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="16" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="B10" s="17">
-        <v>1</v>
+        <v>60</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>36</v>
@@ -4410,103 +4668,111 @@
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="18">
-        <v>3</v>
-      </c>
-      <c r="L11" s="9"/>
+        <v>4</v>
+      </c>
+      <c r="B11" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="18">
+        <v>3</v>
+      </c>
+      <c r="L12" s="9"/>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="A13" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="17">
+      <c r="B13" s="17">
         <v>-25.5</v>
       </c>
-      <c r="L12" s="9"/>
-    </row>
-    <row r="13" spans="1:19" ht="13.5" thickBot="1">
-      <c r="A13" s="19" t="s">
+      <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="1:19" ht="15" thickBot="1">
+      <c r="A14" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="20">
+      <c r="B14" s="20">
         <v>25.5</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="9"/>
-    </row>
-    <row r="14" spans="1:19" ht="12.75" customHeight="1">
-      <c r="A14" s="42" t="s">
+      <c r="C14" s="12"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="9"/>
+    </row>
+    <row r="15" spans="1:19" ht="12.75" customHeight="1">
+      <c r="A15" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="43"/>
-      <c r="L14" s="9"/>
-    </row>
-    <row r="15" spans="1:19">
-      <c r="A15" s="44"/>
-      <c r="B15" s="45"/>
+      <c r="B15" s="43"/>
       <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:19">
-      <c r="C16" s="12"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="15"/>
+      <c r="A16" s="44"/>
+      <c r="B16" s="45"/>
       <c r="L16" s="9"/>
     </row>
     <row r="17" spans="3:12">
+      <c r="C17" s="12"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="15"/>
       <c r="L17" s="9"/>
     </row>
     <row r="18" spans="3:12">
       <c r="L18" s="9"/>
     </row>
     <row r="19" spans="3:12">
-      <c r="C19" s="12"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="15"/>
       <c r="L19" s="9"/>
     </row>
-    <row r="22" spans="3:12">
-      <c r="C22" s="12"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="15"/>
-    </row>
-    <row r="25" spans="3:12">
-      <c r="C25" s="12"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="15"/>
+    <row r="20" spans="3:12">
+      <c r="C20" s="12"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="9"/>
+    </row>
+    <row r="23" spans="3:12">
+      <c r="C23" s="12"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="15"/>
+    </row>
+    <row r="26" spans="3:12">
+      <c r="C26" s="12"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -4514,7 +4780,7 @@
     <mergeCell ref="C3:K3"/>
     <mergeCell ref="L3:Q3"/>
     <mergeCell ref="R3:S3"/>
-    <mergeCell ref="A14:B15"/>
+    <mergeCell ref="A15:B16"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="0.75" header="0.5" footer="0.3"/>
@@ -4526,33 +4792,38 @@
 &amp;Z&amp;F\&amp;A&amp;R&amp;"-,Regular"&amp;9Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="35.83203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="21" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="11" customWidth="1"/>
-    <col min="4" max="10" width="10.42578125" style="9" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" style="14" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" style="6" customWidth="1"/>
-    <col min="13" max="16" width="10.42578125" style="9" customWidth="1"/>
-    <col min="17" max="17" width="10.42578125" style="14" customWidth="1"/>
-    <col min="18" max="18" width="22.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.85546875" style="9"/>
+    <col min="3" max="3" width="10.5" style="11" customWidth="1"/>
+    <col min="4" max="10" width="10.5" style="9" customWidth="1"/>
+    <col min="11" max="11" width="10.5" style="14" customWidth="1"/>
+    <col min="12" max="12" width="10.5" style="6" customWidth="1"/>
+    <col min="13" max="16" width="10.5" style="9" customWidth="1"/>
+    <col min="17" max="17" width="10.5" style="14" customWidth="1"/>
+    <col min="18" max="18" width="22.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="25" customFormat="1" ht="15">
+    <row r="1" spans="1:19" s="25" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -4592,7 +4863,7 @@
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
     </row>
-    <row r="3" spans="1:19" ht="15.75">
+    <row r="3" spans="1:19" ht="15">
       <c r="A3" s="40" t="s">
         <v>21</v>
       </c>
@@ -4621,7 +4892,7 @@
       </c>
       <c r="S3" s="39"/>
     </row>
-    <row r="4" spans="1:19" ht="38.25">
+    <row r="4" spans="1:19" ht="42">
       <c r="A4" s="23" t="s">
         <v>28</v>
       </c>
@@ -4734,20 +5005,20 @@
         <v>0</v>
       </c>
       <c r="R5" s="28">
-        <f>MAX(E5:E25,N5:N25)*1.05</f>
+        <f>MAX(E5:E26,N5:N26)*1.05</f>
         <v>35.700000000000003</v>
       </c>
       <c r="S5" s="28">
-        <f>B12</f>
+        <f>B13</f>
         <v>-25.5</v>
       </c>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>37</v>
+      <c r="A6" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="17">
+        <v>4</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>32</v>
@@ -4798,16 +5069,16 @@
         <v>0</v>
       </c>
       <c r="S6" s="28">
-        <f>B12</f>
+        <f>B13</f>
         <v>-25.5</v>
       </c>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="18">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>37</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>33</v>
@@ -4839,16 +5110,16 @@
       <c r="L7" s="9"/>
       <c r="R7" s="28"/>
       <c r="S7" s="28">
-        <f>B13</f>
+        <f>B14</f>
         <v>25.5</v>
       </c>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" s="18">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>34</v>
@@ -4880,16 +5151,16 @@
       <c r="L8" s="9"/>
       <c r="R8" s="28"/>
       <c r="S8" s="28">
-        <f>B13</f>
+        <f>B14</f>
         <v>25.5</v>
       </c>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="17">
-        <v>55</v>
+        <v>3</v>
+      </c>
+      <c r="B9" s="18">
+        <v>100</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>35</v>
@@ -4922,10 +5193,10 @@
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="16" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="B10" s="17">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>36</v>
@@ -4958,103 +5229,111 @@
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="18">
-        <v>3</v>
-      </c>
-      <c r="L11" s="9"/>
+        <v>4</v>
+      </c>
+      <c r="B11" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="18">
+        <v>3</v>
+      </c>
+      <c r="L12" s="9"/>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="A13" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="17">
+      <c r="B13" s="17">
         <v>-25.5</v>
       </c>
-      <c r="L12" s="9"/>
-    </row>
-    <row r="13" spans="1:19" ht="13.5" thickBot="1">
-      <c r="A13" s="19" t="s">
+      <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="1:19" ht="15" thickBot="1">
+      <c r="A14" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="20">
+      <c r="B14" s="20">
         <v>25.5</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="9"/>
-    </row>
-    <row r="14" spans="1:19" ht="12.75" customHeight="1">
-      <c r="A14" s="42" t="s">
+      <c r="C14" s="12"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="9"/>
+    </row>
+    <row r="15" spans="1:19" ht="12.75" customHeight="1">
+      <c r="A15" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="43"/>
-      <c r="L14" s="9"/>
-    </row>
-    <row r="15" spans="1:19">
-      <c r="A15" s="44"/>
-      <c r="B15" s="45"/>
+      <c r="B15" s="43"/>
       <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:19">
-      <c r="C16" s="12"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="15"/>
+      <c r="A16" s="44"/>
+      <c r="B16" s="45"/>
       <c r="L16" s="9"/>
     </row>
     <row r="17" spans="3:12">
+      <c r="C17" s="12"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="15"/>
       <c r="L17" s="9"/>
     </row>
     <row r="18" spans="3:12">
       <c r="L18" s="9"/>
     </row>
     <row r="19" spans="3:12">
-      <c r="C19" s="12"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="15"/>
       <c r="L19" s="9"/>
     </row>
-    <row r="22" spans="3:12">
-      <c r="C22" s="12"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="15"/>
-    </row>
-    <row r="25" spans="3:12">
-      <c r="C25" s="12"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="15"/>
+    <row r="20" spans="3:12">
+      <c r="C20" s="12"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="9"/>
+    </row>
+    <row r="23" spans="3:12">
+      <c r="C23" s="12"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="15"/>
+    </row>
+    <row r="26" spans="3:12">
+      <c r="C26" s="12"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -5062,7 +5341,7 @@
     <mergeCell ref="C3:K3"/>
     <mergeCell ref="L3:Q3"/>
     <mergeCell ref="R3:S3"/>
-    <mergeCell ref="A14:B15"/>
+    <mergeCell ref="A15:B16"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="0.75" header="0.5" footer="0.3"/>
@@ -5074,33 +5353,38 @@
 &amp;Z&amp;F\&amp;A&amp;R&amp;"-,Regular"&amp;9Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="35.83203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="21" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="11" customWidth="1"/>
-    <col min="4" max="10" width="10.42578125" style="9" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" style="14" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" style="6" customWidth="1"/>
-    <col min="13" max="16" width="10.42578125" style="9" customWidth="1"/>
-    <col min="17" max="17" width="10.42578125" style="14" customWidth="1"/>
-    <col min="18" max="18" width="22.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="8.85546875" style="9"/>
+    <col min="3" max="3" width="10.5" style="11" customWidth="1"/>
+    <col min="4" max="10" width="10.5" style="9" customWidth="1"/>
+    <col min="11" max="11" width="10.5" style="14" customWidth="1"/>
+    <col min="12" max="12" width="10.5" style="6" customWidth="1"/>
+    <col min="13" max="16" width="10.5" style="9" customWidth="1"/>
+    <col min="17" max="17" width="10.5" style="14" customWidth="1"/>
+    <col min="18" max="18" width="22.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="25" customFormat="1" ht="15">
+    <row r="1" spans="1:19" s="25" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -5140,7 +5424,7 @@
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
     </row>
-    <row r="3" spans="1:19" ht="15.75">
+    <row r="3" spans="1:19" ht="15">
       <c r="A3" s="40" t="s">
         <v>21</v>
       </c>
@@ -5169,7 +5453,7 @@
       </c>
       <c r="S3" s="39"/>
     </row>
-    <row r="4" spans="1:19" ht="38.25">
+    <row r="4" spans="1:19" ht="42">
       <c r="A4" s="23" t="s">
         <v>28</v>
       </c>
@@ -5282,20 +5566,20 @@
         <v>0</v>
       </c>
       <c r="R5" s="28">
-        <f>MAX(E5:E25,N5:N25)*1.05</f>
+        <f>MAX(E5:E26,N5:N26)*1.05</f>
         <v>35.700000000000003</v>
       </c>
       <c r="S5" s="28">
-        <f>B12</f>
+        <f>B13</f>
         <v>-25.5</v>
       </c>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>37</v>
+      <c r="A6" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="17">
+        <v>5</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>32</v>
@@ -5346,16 +5630,16 @@
         <v>0</v>
       </c>
       <c r="S6" s="28">
-        <f>B12</f>
+        <f>B13</f>
         <v>-25.5</v>
       </c>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="18">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>37</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>33</v>
@@ -5387,16 +5671,16 @@
       <c r="L7" s="9"/>
       <c r="R7" s="28"/>
       <c r="S7" s="28">
-        <f>B13</f>
+        <f>B14</f>
         <v>25.5</v>
       </c>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" s="18">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>34</v>
@@ -5428,16 +5712,16 @@
       <c r="L8" s="9"/>
       <c r="R8" s="28"/>
       <c r="S8" s="28">
-        <f>B13</f>
+        <f>B14</f>
         <v>25.5</v>
       </c>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="17">
-        <v>30</v>
+        <v>3</v>
+      </c>
+      <c r="B9" s="18">
+        <v>100</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>35</v>
@@ -5470,10 +5754,10 @@
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="16" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="B10" s="17">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>36</v>
@@ -5506,103 +5790,111 @@
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="18">
-        <v>3</v>
-      </c>
-      <c r="L11" s="9"/>
+        <v>4</v>
+      </c>
+      <c r="B11" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="18">
+        <v>3</v>
+      </c>
+      <c r="L12" s="9"/>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="A13" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="17">
+      <c r="B13" s="17">
         <v>-25.5</v>
       </c>
-      <c r="L12" s="9"/>
-    </row>
-    <row r="13" spans="1:19" ht="13.5" thickBot="1">
-      <c r="A13" s="19" t="s">
+      <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="1:19" ht="15" thickBot="1">
+      <c r="A14" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="20">
+      <c r="B14" s="20">
         <v>25.5</v>
       </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="9"/>
-    </row>
-    <row r="14" spans="1:19" ht="12.75" customHeight="1">
-      <c r="A14" s="42" t="s">
+      <c r="C14" s="12"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="9"/>
+    </row>
+    <row r="15" spans="1:19" ht="12.75" customHeight="1">
+      <c r="A15" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="43"/>
-      <c r="L14" s="9"/>
-    </row>
-    <row r="15" spans="1:19">
-      <c r="A15" s="44"/>
-      <c r="B15" s="45"/>
+      <c r="B15" s="43"/>
       <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:19">
-      <c r="C16" s="12"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="15"/>
+      <c r="A16" s="44"/>
+      <c r="B16" s="45"/>
       <c r="L16" s="9"/>
     </row>
     <row r="17" spans="3:12">
+      <c r="C17" s="12"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="15"/>
       <c r="L17" s="9"/>
     </row>
     <row r="18" spans="3:12">
       <c r="L18" s="9"/>
     </row>
     <row r="19" spans="3:12">
-      <c r="C19" s="12"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="15"/>
       <c r="L19" s="9"/>
     </row>
-    <row r="22" spans="3:12">
-      <c r="C22" s="12"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="15"/>
-    </row>
-    <row r="25" spans="3:12">
-      <c r="C25" s="12"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="15"/>
+    <row r="20" spans="3:12">
+      <c r="C20" s="12"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="9"/>
+    </row>
+    <row r="23" spans="3:12">
+      <c r="C23" s="12"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="15"/>
+    </row>
+    <row r="26" spans="3:12">
+      <c r="C26" s="12"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -5610,7 +5902,7 @@
     <mergeCell ref="C3:K3"/>
     <mergeCell ref="L3:Q3"/>
     <mergeCell ref="R3:S3"/>
-    <mergeCell ref="A14:B15"/>
+    <mergeCell ref="A15:B16"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="0.75" header="0.5" footer="0.3"/>
@@ -5622,33 +5914,38 @@
 &amp;Z&amp;F\&amp;A&amp;R&amp;"-,Regular"&amp;9Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="41.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="11" customWidth="1"/>
-    <col min="4" max="10" width="10.5703125" style="9" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" style="14" customWidth="1"/>
-    <col min="12" max="12" width="10.5703125" style="6" customWidth="1"/>
-    <col min="13" max="16" width="10.5703125" style="9" customWidth="1"/>
-    <col min="17" max="17" width="10.5703125" style="34" customWidth="1"/>
-    <col min="18" max="18" width="22.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="36.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="11" customWidth="1"/>
+    <col min="4" max="10" width="10.5" style="9" customWidth="1"/>
+    <col min="11" max="11" width="10.5" style="14" customWidth="1"/>
+    <col min="12" max="12" width="10.5" style="6" customWidth="1"/>
+    <col min="13" max="16" width="10.5" style="9" customWidth="1"/>
+    <col min="17" max="17" width="10.5" style="34" customWidth="1"/>
+    <col min="18" max="18" width="22.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" ht="15">
+    <row r="1" spans="1:19" s="1" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -5658,7 +5955,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="30" customFormat="1" ht="15.75">
+    <row r="3" spans="1:19" s="30" customFormat="1" ht="15">
       <c r="A3" s="40" t="s">
         <v>21</v>
       </c>
@@ -5687,7 +5984,7 @@
       </c>
       <c r="S3" s="46"/>
     </row>
-    <row r="4" spans="1:19" ht="38.25">
+    <row r="4" spans="1:19" ht="42">
       <c r="A4" s="31"/>
       <c r="B4" s="31"/>
       <c r="C4" s="22" t="s">
@@ -5795,20 +6092,20 @@
         <v>0</v>
       </c>
       <c r="R5" s="35">
-        <f>MAX(E5:E25,N5:N25)*1.05</f>
+        <f>MAX(E5:E26,N5:N26)*1.05</f>
         <v>57.928500000000007</v>
       </c>
       <c r="S5" s="35">
-        <f>B12</f>
+        <f>B13</f>
         <v>-50</v>
       </c>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="17" t="s">
-        <v>47</v>
+      <c r="A6" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6" s="17">
+        <v>6</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>48</v>
@@ -5859,16 +6156,16 @@
         <v>0</v>
       </c>
       <c r="S6" s="35">
-        <f>B12</f>
+        <f>B13</f>
         <v>-50</v>
       </c>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="18">
-        <v>60</v>
+        <v>1</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>47</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>49</v>
@@ -5900,16 +6197,16 @@
       <c r="L7" s="9"/>
       <c r="R7" s="35"/>
       <c r="S7" s="35">
-        <f>B13</f>
+        <f>B14</f>
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:19">
       <c r="A8" s="16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" s="18">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>33</v>
@@ -5941,16 +6238,16 @@
       <c r="L8" s="9"/>
       <c r="R8" s="35"/>
       <c r="S8" s="35">
-        <f>B13</f>
+        <f>B14</f>
         <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="17">
-        <v>150</v>
+        <v>3</v>
+      </c>
+      <c r="B9" s="18">
+        <v>100</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>31</v>
@@ -5983,10 +6280,10 @@
     </row>
     <row r="10" spans="1:19">
       <c r="A10" s="16" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="B10" s="17">
-        <v>1</v>
+        <v>150</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>32</v>
@@ -6019,10 +6316,10 @@
     </row>
     <row r="11" spans="1:19">
       <c r="A11" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="18">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="B11" s="17">
+        <v>1</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>51</v>
@@ -6055,10 +6352,10 @@
     </row>
     <row r="12" spans="1:19">
       <c r="A12" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="17">
-        <v>-50</v>
+        <v>6</v>
+      </c>
+      <c r="B12" s="18">
+        <v>3</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>52</v>
@@ -6089,12 +6386,12 @@
       </c>
       <c r="L12" s="9"/>
     </row>
-    <row r="13" spans="1:19" ht="13.5" thickBot="1">
-      <c r="A13" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="20">
-        <v>50</v>
+    <row r="13" spans="1:19">
+      <c r="A13" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="17">
+        <v>-50</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>53</v>
@@ -6125,63 +6422,71 @@
       </c>
       <c r="L13" s="9"/>
     </row>
-    <row r="14" spans="1:19">
-      <c r="L14" s="9"/>
+    <row r="14" spans="1:19" ht="15" thickBot="1">
+      <c r="A14" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="20">
+        <v>50</v>
+      </c>
     </row>
     <row r="15" spans="1:19">
       <c r="L15" s="9"/>
     </row>
     <row r="16" spans="1:19">
-      <c r="C16" s="12"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="15"/>
       <c r="L16" s="9"/>
     </row>
     <row r="17" spans="3:12">
+      <c r="C17" s="12"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="15"/>
       <c r="L17" s="9"/>
     </row>
     <row r="18" spans="3:12">
       <c r="L18" s="9"/>
     </row>
     <row r="19" spans="3:12">
-      <c r="C19" s="12"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="15"/>
       <c r="L19" s="9"/>
     </row>
-    <row r="22" spans="3:12">
-      <c r="C22" s="12"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="15"/>
-    </row>
-    <row r="25" spans="3:12">
-      <c r="C25" s="12"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="15"/>
+    <row r="20" spans="3:12">
+      <c r="C20" s="12"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="9"/>
+    </row>
+    <row r="23" spans="3:12">
+      <c r="C23" s="12"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="15"/>
+    </row>
+    <row r="26" spans="3:12">
+      <c r="C26" s="12"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -6192,13 +6497,18 @@
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="0.75" header="0.5" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddHeader xml:space="preserve">&amp;L&amp;"-,Regular"&amp;9Draft&amp;C&amp;"Times New Roman,Bold"&amp;11 </oddHeader>
     <oddFooter>&amp;L&amp;K4D4D4DG&amp;8RADIENT&amp;"Cambria,Regular"&amp;6
 &amp;"-,Regular"&amp;K4D4D4D
 &amp;Z&amp;F\&amp;A&amp;R&amp;"-,Regular"&amp;9Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>